<commit_message>
Rework all classes to convert OD pair in ODP entity (disaggregate origin-destination pairs in origin-destination-product category entities). Parameters and other parts of the logic of the model may still need to be modified.
</commit_message>
<xml_diff>
--- a/data/railway_od_pairs.xlsx
+++ b/data/railway_od_pairs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="137">
   <si>
     <t>30-45</t>
   </si>
@@ -426,13 +426,24 @@
   <si>
     <t>3-43</t>
   </si>
+  <si>
+    <t>railway_category</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -460,11 +471,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -775,1325 +791,2203 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>15</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="D1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3">
-        <v>66520.254000000001</v>
+        <v>127540.52073273997</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
       </c>
       <c r="D2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>130</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3">
-        <v>5000</v>
+        <v>29141.286038496473</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
       </c>
       <c r="D3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3">
-        <v>547800</v>
+        <v>37816</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
       </c>
       <c r="D4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3">
-        <v>75000</v>
+        <v>35481.353006894577</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
       </c>
       <c r="D5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3">
-        <v>34100</v>
+        <v>9068.9813571231753</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
       </c>
       <c r="D6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3">
-        <v>56100</v>
+        <v>66178</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
       </c>
       <c r="D7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>117</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3">
-        <v>25300</v>
+        <v>33217.576403841915</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
       </c>
       <c r="D8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>96</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3">
-        <v>56100</v>
+        <v>13119.245591411502</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
       </c>
       <c r="D9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3">
-        <v>145846.28692429207</v>
+        <v>93185.75</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
       </c>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3">
-        <v>77011.194000000003</v>
+        <v>37343.200000000004</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
       </c>
       <c r="D11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B12" s="3">
-        <v>15928.499999999998</v>
+        <v>42403.198614379697</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
       </c>
       <c r="D12"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3">
-        <v>57200</v>
+        <v>29281.503377839501</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
       </c>
       <c r="D13"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B14" s="3">
-        <v>174709.43579285187</v>
+        <v>65350.6</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
       </c>
       <c r="D14"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="B15" s="3">
-        <v>96800</v>
+        <v>68801.596510717645</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1</v>
       </c>
       <c r="D15"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="B16" s="3">
-        <v>216467.29</v>
+        <v>99894.503913999608</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1</v>
       </c>
       <c r="D16"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B17" s="3">
-        <v>419624.182400044</v>
+        <v>65936.829161201429</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1</v>
       </c>
       <c r="D17"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="B18" s="3">
-        <v>185524.46</v>
+        <v>212671.9</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1</v>
       </c>
       <c r="D18"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="B19" s="3">
-        <v>49975.902000000002</v>
+        <v>67508.67747857995</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>124</v>
+        <v>22</v>
       </c>
       <c r="B20" s="3">
-        <v>11914</v>
+        <v>213188.01872256826</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B21" s="3">
-        <v>1067634.1141672351</v>
+        <v>55978.568292450909</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>106</v>
+        <v>23</v>
       </c>
       <c r="B22" s="3">
-        <v>41000</v>
+        <v>71045.437236189377</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="B23" s="3">
-        <v>75000</v>
+        <v>44509.516262606776</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>118</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3">
-        <v>22100</v>
+        <v>191779.62637205271</v>
+      </c>
+      <c r="C24" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3">
-        <v>1056188</v>
+        <v>258296.192952385</v>
+      </c>
+      <c r="C25" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3">
-        <v>52187.514999999999</v>
+        <v>104890</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B27" s="3">
-        <v>743803.17746560939</v>
+        <v>152639.10532840685</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="B28" s="3">
-        <v>16732.468000000001</v>
+        <v>137858.63226857415</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="B29" s="3">
-        <v>544966.78</v>
+        <v>47130.70440228939</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="B30" s="3">
-        <v>100465.79</v>
+        <v>201995.06655613636</v>
+      </c>
+      <c r="C30" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="B31" s="3">
-        <v>176700.57</v>
+        <v>144958.41277428553</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="3">
+        <v>30420.800000000003</v>
+      </c>
+      <c r="C32" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="3">
+        <v>20596.627243388237</v>
+      </c>
+      <c r="C33" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="3">
+        <v>41592.459680903834</v>
+      </c>
+      <c r="C34" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="3">
+        <v>53236.399999999994</v>
+      </c>
+      <c r="C35" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="3">
+        <v>116682.87752585208</v>
+      </c>
+      <c r="C36" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="3">
+        <v>205678.75</v>
+      </c>
+      <c r="C37" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="3">
+        <v>112528.15499452136</v>
+      </c>
+      <c r="C38" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="3">
+        <v>72304</v>
+      </c>
+      <c r="C39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="3">
+        <v>83486.974537763585</v>
+      </c>
+      <c r="C40" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="3">
+        <v>16826.122601439787</v>
+      </c>
+      <c r="C41" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="3">
+        <v>90380</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="3">
+        <v>173176.64013155986</v>
+      </c>
+      <c r="C43" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="3">
+        <v>95477.001351254483</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="3">
+        <v>124560.47698791185</v>
+      </c>
+      <c r="C45" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="3">
+        <v>152639.10532840685</v>
+      </c>
+      <c r="C46" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="3">
+        <v>146521.14947738417</v>
+      </c>
+      <c r="C47" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="3">
+        <v>55781.748168259932</v>
+      </c>
+      <c r="C48" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="3">
+        <v>39612.484515818447</v>
+      </c>
+      <c r="C49" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="3">
+        <v>132928.49140242304</v>
+      </c>
+      <c r="C50" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="3">
+        <v>17537.295581713413</v>
+      </c>
+      <c r="C51" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B52" s="3">
+        <v>35762.163434948634</v>
+      </c>
+      <c r="C52" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B53" s="3">
+        <v>153087.23278307472</v>
+      </c>
+      <c r="C53" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B54" s="3">
+        <v>35762.163434948663</v>
+      </c>
+      <c r="C54" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="3">
+        <v>410144.22725310811</v>
+      </c>
+      <c r="C55" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="3">
+        <v>238969.13590303698</v>
+      </c>
+      <c r="C56" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57" s="3">
+        <v>32586</v>
+      </c>
+      <c r="C57" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58" s="3">
+        <v>101400.90158853697</v>
+      </c>
+      <c r="C58" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B59" s="3">
+        <v>48615.600000000006</v>
+      </c>
+      <c r="C59" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B60" s="3">
+        <v>234270.38837124861</v>
+      </c>
+      <c r="C60" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B61" s="3">
+        <v>244444.90868565158</v>
+      </c>
+      <c r="C61" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B62" s="3">
+        <v>26718.876238633235</v>
+      </c>
+      <c r="C62" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" s="3">
+        <v>292837.96762648539</v>
+      </c>
+      <c r="C63" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" s="3">
+        <v>79813.308256947086</v>
+      </c>
+      <c r="C64" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B65" s="3">
+        <v>16634.400000000001</v>
+      </c>
+      <c r="C65" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B66" s="3">
+        <v>94968.612065456342</v>
+      </c>
+      <c r="C66" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B67" s="3">
+        <v>335584.52129543561</v>
+      </c>
+      <c r="C67" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B68" s="3">
+        <v>58754.554557901625</v>
+      </c>
+      <c r="C68" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B69" s="3">
+        <v>415671.11832148652</v>
+      </c>
+      <c r="C69" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B70" s="3">
+        <v>71279.044416608842</v>
+      </c>
+      <c r="C70" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B71" s="3">
+        <v>118710.76508182043</v>
+      </c>
+      <c r="C71" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="3">
+        <v>15928.499999999998</v>
+      </c>
+      <c r="C72" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B73" s="3">
+        <v>21436.052816368221</v>
+      </c>
+      <c r="C73" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B74" s="3">
+        <v>45612.352414952475</v>
+      </c>
+      <c r="C74" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B75" s="3">
+        <v>522320.76434067497</v>
+      </c>
+      <c r="C75" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B76" s="3">
+        <v>104275.06542306861</v>
+      </c>
+      <c r="C76" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B77" s="3">
+        <v>21436.052816368232</v>
+      </c>
+      <c r="C77" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B78" s="3">
+        <v>19508</v>
+      </c>
+      <c r="C78" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B79" s="3">
+        <v>19508</v>
+      </c>
+      <c r="C79" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B80" s="3">
+        <v>130197.86528291726</v>
+      </c>
+      <c r="C80" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B81" s="3">
+        <v>14262.918822015883</v>
+      </c>
+      <c r="C81" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B82" s="3">
+        <v>268812.21523172566</v>
+      </c>
+      <c r="C82" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B83" s="3">
+        <v>317614</v>
+      </c>
+      <c r="C83" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B84" s="3">
+        <v>353002.61416723503</v>
+      </c>
+      <c r="C84" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B85" s="3">
+        <v>397017.5</v>
+      </c>
+      <c r="C85" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="3">
+        <v>118853.04204314978</v>
+      </c>
+      <c r="C86" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B87" s="3">
+        <v>18062.983557381482</v>
+      </c>
+      <c r="C87" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88" s="3">
+        <v>142862.46877182633</v>
+      </c>
+      <c r="C88" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B89" s="3">
+        <v>74716.635230199157</v>
+      </c>
+      <c r="C89" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B90" s="3">
+        <v>174709.43579285187</v>
+      </c>
+      <c r="C90" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B91" s="3">
+        <v>139761.87565104209</v>
+      </c>
+      <c r="C91" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B92" s="3">
+        <v>469086.70666041004</v>
+      </c>
+      <c r="C92" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B93" s="3">
+        <v>82724.929167692113</v>
+      </c>
+      <c r="C93" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B94" s="3">
+        <v>191991.54163750727</v>
+      </c>
+      <c r="C94" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="3">
-        <v>77544.691136702953</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="B95" s="3">
+        <v>37088.48457993153</v>
+      </c>
+      <c r="C95" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B96" s="3">
+        <v>3367.7219768398677</v>
+      </c>
+      <c r="C96" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B97" s="3">
+        <v>37088.484579931552</v>
+      </c>
+      <c r="C97" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B98" s="3">
+        <v>5849.0172573820937</v>
+      </c>
+      <c r="C98" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B99" s="3">
+        <v>378193.7991551407</v>
+      </c>
+      <c r="C99" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B100" s="3">
+        <v>41430.383244903285</v>
+      </c>
+      <c r="C100" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B101" s="3">
+        <v>1760200</v>
+      </c>
+      <c r="C101" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B102" s="3">
+        <v>1056188</v>
+      </c>
+      <c r="C102" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B103" s="3">
+        <v>747500</v>
+      </c>
+      <c r="C103" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B104" s="3">
+        <v>547800</v>
+      </c>
+      <c r="C104" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B105" s="3">
+        <v>544966.78</v>
+      </c>
+      <c r="C105" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B106" s="3">
+        <v>525676.78</v>
+      </c>
+      <c r="C106" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B107" s="3">
+        <v>471153.64</v>
+      </c>
+      <c r="C107" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B108" s="3">
+        <v>443300</v>
+      </c>
+      <c r="C108" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B109" s="3">
+        <v>420390.21</v>
+      </c>
+      <c r="C109" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B110" s="3">
+        <v>417600</v>
+      </c>
+      <c r="C110" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B111" s="3">
+        <v>379269.4</v>
+      </c>
+      <c r="C111" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B112" s="3">
+        <v>369953.46</v>
+      </c>
+      <c r="C112" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B113" s="3">
+        <v>277638.37</v>
+      </c>
+      <c r="C113" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B114" s="3">
+        <v>270832.71000000002</v>
+      </c>
+      <c r="C114" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B115" s="3">
+        <v>266533.21999999997</v>
+      </c>
+      <c r="C115" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B116" s="3">
+        <v>263200</v>
+      </c>
+      <c r="C116" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B117" s="3">
+        <v>240000</v>
+      </c>
+      <c r="C117" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B118" s="3">
+        <v>227700</v>
+      </c>
+      <c r="C118" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B119" s="3">
+        <v>225366.86</v>
+      </c>
+      <c r="C119" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B120" s="3">
+        <v>216467.29</v>
+      </c>
+      <c r="C120" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B121" s="3">
+        <v>198197.5</v>
+      </c>
+      <c r="C121" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B122" s="3">
+        <v>190000</v>
+      </c>
+      <c r="C122" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B123" s="3">
+        <v>185524.46</v>
+      </c>
+      <c r="C123" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B124" s="3">
+        <v>181979.39</v>
+      </c>
+      <c r="C124" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B125" s="3">
+        <v>176700.57</v>
+      </c>
+      <c r="C125" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B126" s="3">
+        <v>170000</v>
+      </c>
+      <c r="C126" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B127" s="3">
+        <v>163224.34</v>
+      </c>
+      <c r="C127" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B128" s="3">
+        <v>150000</v>
+      </c>
+      <c r="C128" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B129" s="3">
+        <v>147184.04999999999</v>
+      </c>
+      <c r="C129" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B130" s="3">
+        <v>132715.46</v>
+      </c>
+      <c r="C130" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B131" s="3">
+        <v>125359.69</v>
+      </c>
+      <c r="C131" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B132" s="3">
+        <v>104500</v>
+      </c>
+      <c r="C132" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B133" s="3">
+        <v>100465.79</v>
+      </c>
+      <c r="C133" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B134" s="3">
+        <v>100000</v>
+      </c>
+      <c r="C134" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B135" s="3">
+        <v>96800</v>
+      </c>
+      <c r="C135" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B136" s="3">
+        <v>90523.971999999994</v>
+      </c>
+      <c r="C136" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B137" s="3">
+        <v>87500</v>
+      </c>
+      <c r="C137" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B138" s="3">
+        <v>81794.334000000003</v>
+      </c>
+      <c r="C138" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B139" s="3">
+        <v>77500</v>
+      </c>
+      <c r="C139" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B140" s="3">
+        <v>77011.194000000003</v>
+      </c>
+      <c r="C140" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B141" s="3">
+        <v>77010</v>
+      </c>
+      <c r="C141" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B142" s="3">
+        <v>75118.187000000005</v>
+      </c>
+      <c r="C142" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B143" s="3">
+        <v>75016</v>
+      </c>
+      <c r="C143" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B144" s="3">
+        <v>75000</v>
+      </c>
+      <c r="C144" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B145" s="3">
+        <v>75000</v>
+      </c>
+      <c r="C145" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B146" s="3">
+        <v>66520.254000000001</v>
+      </c>
+      <c r="C146" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B147" s="3">
+        <v>63500</v>
+      </c>
+      <c r="C147" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B148" s="3">
+        <v>62500</v>
+      </c>
+      <c r="C148" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B149" s="3">
+        <v>62142.519</v>
+      </c>
+      <c r="C149" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B150" s="3">
+        <v>60366.972000000002</v>
+      </c>
+      <c r="C150" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B151" s="3">
+        <v>58044.334000000003</v>
+      </c>
+      <c r="C151" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B152" s="3">
+        <v>57250</v>
+      </c>
+      <c r="C152" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B153" s="3">
+        <v>57200</v>
+      </c>
+      <c r="C153" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B154" s="3">
+        <v>56100</v>
+      </c>
+      <c r="C154" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B155" s="3">
+        <v>56100</v>
+      </c>
+      <c r="C155" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B156" s="3">
+        <v>52187.514999999999</v>
+      </c>
+      <c r="C156" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B157" s="3">
+        <v>52000</v>
+      </c>
+      <c r="C157" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B158" s="3">
+        <v>49975.902000000002</v>
+      </c>
+      <c r="C158" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B159" s="3">
+        <v>49000</v>
+      </c>
+      <c r="C159" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B160" s="3">
+        <v>47284.544000000002</v>
+      </c>
+      <c r="C160" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B161" s="3">
+        <v>46485.449000000001</v>
+      </c>
+      <c r="C161" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B162" s="3">
+        <v>45068.192999999999</v>
+      </c>
+      <c r="C162" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B163" s="3">
         <v>43710.050999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="3">
-        <v>715080.2878114325</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" s="3">
-        <v>147184.04999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="C163" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B164" s="3">
+        <v>42133.027999999998</v>
+      </c>
+      <c r="C164" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B165" s="3">
+        <v>41000</v>
+      </c>
+      <c r="C165" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B166" s="3">
+        <v>39490</v>
+      </c>
+      <c r="C166" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B167" s="3">
+        <v>36500</v>
+      </c>
+      <c r="C167" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B168" s="3">
+        <v>36261.805999999997</v>
+      </c>
+      <c r="C168" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B169" s="3">
+        <v>36000</v>
+      </c>
+      <c r="C169" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B170" s="3">
+        <v>35500</v>
+      </c>
+      <c r="C170" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B171" s="3">
         <v>34648.453999999998</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="3">
-        <v>39016</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B38" s="3">
-        <v>32586</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="3">
-        <v>16634.400000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" s="3">
-        <v>224611.55965297201</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" s="3">
-        <v>337628.44199927041</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="3">
-        <v>346953.47933042189</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" s="3">
-        <v>649113.36315614509</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B44" s="3">
-        <v>150016.50158853698</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B45" s="3">
-        <v>75016</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B46" s="3">
-        <v>198197.5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B47" s="3">
-        <v>747500</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B48" s="3">
-        <v>266533.21999999997</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B49" s="3">
-        <v>49000</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B50" s="3">
-        <v>225366.86</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="C171" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B172" s="3">
+        <v>34100</v>
+      </c>
+      <c r="C172" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B173" s="3">
+        <v>33500</v>
+      </c>
+      <c r="C173" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B174" s="3">
+        <v>31250</v>
+      </c>
+      <c r="C174" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B175" s="3">
+        <v>30000</v>
+      </c>
+      <c r="C175" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B176" s="3">
+        <v>25300</v>
+      </c>
+      <c r="C176" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B177" s="3">
+        <v>22100</v>
+      </c>
+      <c r="C177" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B178" s="3">
+        <v>20900</v>
+      </c>
+      <c r="C178" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B179" s="3">
+        <v>18700</v>
+      </c>
+      <c r="C179" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B180" s="3">
+        <v>16732.468000000001</v>
+      </c>
+      <c r="C180" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B181" s="3">
+        <v>14679.745999999999</v>
+      </c>
+      <c r="C181" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B182" s="3">
+        <v>13049.767</v>
+      </c>
+      <c r="C182" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B183" s="3">
+        <v>11914</v>
+      </c>
+      <c r="C183" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B184" s="3">
+        <v>11750</v>
+      </c>
+      <c r="C184" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B185" s="3">
+        <v>11750</v>
+      </c>
+      <c r="C185" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B186" s="3">
+        <v>10955.665999999999</v>
+      </c>
+      <c r="C186" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B187" s="3">
+        <v>9500</v>
+      </c>
+      <c r="C187" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B188" s="3">
+        <v>8396.1929999999993</v>
+      </c>
+      <c r="C188" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B189" s="3">
+        <v>5000</v>
+      </c>
+      <c r="C189" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B190" s="3">
+        <v>5000</v>
+      </c>
+      <c r="C190" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B191" s="3">
+        <v>2500</v>
+      </c>
+      <c r="C191" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B192" s="3">
+        <v>2167.2865000000002</v>
+      </c>
+      <c r="C192" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B193" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C193" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B194" s="3">
         <v>919.64323999999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B52" s="3">
-        <v>132715.46</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B53" s="3">
-        <v>47284.544000000002</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B54" s="3">
-        <v>170000</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B55" s="3">
-        <v>268653.64148281433</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B56" s="3">
-        <v>263200</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B57" s="3">
-        <v>479502.47996196279</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="C194" s="4">
         <v>4</v>
       </c>
-      <c r="B58" s="3">
-        <v>217579.1040020255</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B59" s="3">
-        <v>36000</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B60" s="3">
-        <v>150465.78698413644</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" s="3">
-        <v>240000</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B62" s="3">
-        <v>52000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B63" s="3">
-        <v>62142.519</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B64" s="3">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B65" s="3">
-        <v>77500</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B66" s="3">
-        <v>136916.02560053125</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B67" s="3">
-        <v>75118.187000000005</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B68" s="3">
-        <v>5849.0172573820937</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B69" s="3">
-        <v>379269.4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B70" s="3">
-        <v>139761.87565104209</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B71" s="3">
-        <v>90523.971999999994</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B72" s="3">
-        <v>42133.027999999998</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B73" s="3">
-        <v>14679.745999999999</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B74" s="3">
-        <v>13049.767</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B75" s="3">
-        <v>104890</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B76" s="3">
-        <v>213188.01872256826</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B77" s="3">
-        <v>163224.34</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B78" s="3">
-        <v>77010</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B79" s="3">
-        <v>8396.1929999999993</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B80" s="3">
-        <v>258296.192952385</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B81" s="3">
-        <v>2167.2865000000002</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B82" s="3">
-        <v>39612.484515818447</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B83" s="3">
-        <v>11750</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B84" s="3">
-        <v>11750</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B85" s="3">
-        <v>62500</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B86" s="3">
-        <v>33500</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B87" s="3">
-        <v>322361.62752585206</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B88" s="3">
-        <v>277638.37</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B89" s="3">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B90" s="3">
-        <v>45068.192999999999</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B91" s="3">
-        <v>9500</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B92" s="3">
-        <v>39490</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B93" s="3">
-        <v>413272.9993366588</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B94" s="3">
-        <v>36261.805999999997</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B95" s="3">
-        <v>1094968.6157387095</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B96" s="3">
-        <v>270832.71000000002</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B97" s="3">
-        <v>262997.09713920334</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B98" s="3">
-        <v>417600</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B99" s="3">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B100" s="3">
-        <v>878085.44917896588</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B101" s="3">
-        <v>46485.449000000001</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B102" s="3">
-        <v>67508.67747857995</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B103" s="3">
-        <v>363313.14816329977</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B104" s="3">
-        <v>125359.69</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B105" s="3">
-        <v>369953.46</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B106" s="3">
-        <v>174378.50199221919</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B107" s="3">
-        <v>35500</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B108" s="3">
-        <v>148544.33436401776</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B109" s="3">
-        <v>58044.334000000003</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B110" s="3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B111" s="3">
-        <v>447304.82958591869</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B112" s="3">
-        <v>81794.334000000003</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B113" s="3">
-        <v>227700</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B114" s="3">
-        <v>10955.665999999999</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B115" s="3">
-        <v>104500</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B116" s="3">
-        <v>18700</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B117" s="3">
-        <v>20900</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B118" s="3">
-        <v>112528.15499452136</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B119" s="3">
-        <v>443300</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B120" s="3">
-        <v>57250</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B121" s="3">
-        <v>31250</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B122" s="3">
-        <v>36500</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B123" s="3">
-        <v>156681.80677123644</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B124" s="3">
-        <v>525676.78</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B125" s="3">
-        <v>420390.21</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B126" s="3">
-        <v>139522.57199525341</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B127" s="3">
-        <v>471153.64</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B128" s="3">
-        <v>87500</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B129" s="3">
-        <v>190000</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B130" s="3">
-        <v>60366.972000000002</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B131" s="3">
-        <v>181979.39</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B132" s="3">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B133" s="3">
-        <v>63500</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B134" s="3">
-        <v>1760200</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B135" s="3">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="3"/>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="3"/>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="3"/>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B139" s="3"/>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="3"/>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B141" s="3"/>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B142" s="3"/>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B143" s="3"/>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B144" s="3"/>
-    </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B145" s="3"/>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B146" s="3"/>
-    </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B147" s="3"/>
-    </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B148" s="3"/>
-    </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B149" s="3"/>
-    </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B150" s="3"/>
-    </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" s="3"/>
-    </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B152" s="3"/>
-    </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" s="3"/>
-    </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B154" s="3"/>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B155" s="3"/>
-    </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B156" s="3"/>
-    </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B157" s="3"/>
-    </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B158" s="3"/>
-    </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B159" s="3"/>
-    </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B160" s="3"/>
-    </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B161" s="3"/>
-    </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B162" s="3"/>
-    </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B163" s="3"/>
-    </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B164" s="3"/>
-    </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B165" s="3"/>
-    </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B166" s="3"/>
-    </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B167" s="3"/>
-    </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B168" s="3"/>
-    </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B169" s="3"/>
-    </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B170" s="3"/>
-    </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B171" s="3"/>
-    </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B172" s="3"/>
-    </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B173" s="3"/>
-    </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B174" s="3"/>
-    </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B175" s="3"/>
-    </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B176" s="3"/>
-    </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B177" s="3"/>
-    </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B178" s="3"/>
-    </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B179" s="3"/>
-    </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B180" s="3"/>
-    </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B181" s="3"/>
-    </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B182" s="3"/>
-    </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B183" s="3"/>
-    </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B184" s="3"/>
-    </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B185" s="3"/>
-    </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B186" s="3"/>
-    </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B187" s="3"/>
-    </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B188" s="3"/>
-    </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B189" s="3"/>
-    </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B190" s="3"/>
-    </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B191" s="3"/>
-    </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B192" s="3"/>
-    </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B193" s="3"/>
-    </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B194" s="3"/>
-    </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B195" s="3"/>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B196" s="3"/>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B197" s="3"/>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B198" s="3"/>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B199" s="3"/>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B200" s="3"/>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B201" s="3"/>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B202" s="3"/>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B203" s="3"/>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B204" s="3"/>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B205" s="3"/>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B206" s="3"/>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B207" s="3"/>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B208" s="3"/>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix bug when loading OD pairs. Remove old reports.
</commit_message>
<xml_diff>
--- a/data/railway_od_pairs.xlsx
+++ b/data/railway_od_pairs.xlsx
@@ -782,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5304"/>
+  <dimension ref="A1:H5304"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,6 +1022,7 @@
       <c r="C19" s="4">
         <v>1</v>
       </c>
+      <c r="D19"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1033,6 +1034,7 @@
       <c r="C20" s="4">
         <v>1</v>
       </c>
+      <c r="D20"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1044,6 +1046,7 @@
       <c r="C21" s="4">
         <v>1</v>
       </c>
+      <c r="D21"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1055,6 +1058,7 @@
       <c r="C22" s="4">
         <v>1</v>
       </c>
+      <c r="D22"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1066,6 +1070,7 @@
       <c r="C23" s="4">
         <v>1</v>
       </c>
+      <c r="D23"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1077,6 +1082,7 @@
       <c r="C24" s="4">
         <v>1</v>
       </c>
+      <c r="D24"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -1088,6 +1094,7 @@
       <c r="C25" s="4">
         <v>1</v>
       </c>
+      <c r="D25"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1099,6 +1106,7 @@
       <c r="C26" s="4">
         <v>1</v>
       </c>
+      <c r="D26"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -1110,6 +1118,7 @@
       <c r="C27" s="4">
         <v>1</v>
       </c>
+      <c r="D27"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -1121,6 +1130,7 @@
       <c r="C28" s="4">
         <v>1</v>
       </c>
+      <c r="D28"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -1132,6 +1142,7 @@
       <c r="C29" s="4">
         <v>1</v>
       </c>
+      <c r="D29"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -1143,6 +1154,7 @@
       <c r="C30" s="4">
         <v>1</v>
       </c>
+      <c r="D30"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -1154,6 +1166,7 @@
       <c r="C31" s="4">
         <v>1</v>
       </c>
+      <c r="D31"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
@@ -1165,8 +1178,9 @@
       <c r="C32" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>13</v>
       </c>
@@ -1176,8 +1190,9 @@
       <c r="C33" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>13</v>
       </c>
@@ -1187,8 +1202,9 @@
       <c r="C34" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>13</v>
       </c>
@@ -1198,8 +1214,9 @@
       <c r="C35" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>26</v>
       </c>
@@ -1209,8 +1226,9 @@
       <c r="C36" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>26</v>
       </c>
@@ -1220,8 +1238,9 @@
       <c r="C37" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>27</v>
       </c>
@@ -1231,8 +1250,9 @@
       <c r="C38" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>28</v>
       </c>
@@ -1242,8 +1262,9 @@
       <c r="C39" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>28</v>
       </c>
@@ -1253,8 +1274,9 @@
       <c r="C40" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>28</v>
       </c>
@@ -1264,8 +1286,9 @@
       <c r="C41" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>28</v>
       </c>
@@ -1275,8 +1298,9 @@
       <c r="C42" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>6</v>
       </c>
@@ -1286,8 +1310,9 @@
       <c r="C43" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>6</v>
       </c>
@@ -1297,8 +1322,9 @@
       <c r="C44" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
@@ -1308,8 +1334,9 @@
       <c r="C45" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>5</v>
       </c>
@@ -1319,8 +1346,9 @@
       <c r="C46" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>5</v>
       </c>
@@ -1330,8 +1358,9 @@
       <c r="C47" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>5</v>
       </c>
@@ -1341,8 +1370,9 @@
       <c r="C48" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>29</v>
       </c>
@@ -1352,8 +1382,9 @@
       <c r="C49" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
@@ -1363,8 +1394,9 @@
       <c r="C50" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>3</v>
       </c>
@@ -1374,8 +1406,9 @@
       <c r="C51" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>30</v>
       </c>
@@ -1385,8 +1418,9 @@
       <c r="C52" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>30</v>
       </c>
@@ -1396,8 +1430,9 @@
       <c r="C53" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>30</v>
       </c>
@@ -1407,8 +1442,9 @@
       <c r="C54" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
@@ -1418,8 +1454,9 @@
       <c r="C55" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -1429,8 +1466,9 @@
       <c r="C56" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>31</v>
       </c>
@@ -1440,8 +1478,9 @@
       <c r="C57" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>32</v>
       </c>
@@ -1451,8 +1490,9 @@
       <c r="C58" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>32</v>
       </c>
@@ -1462,8 +1502,9 @@
       <c r="C59" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>33</v>
       </c>
@@ -1473,8 +1514,9 @@
       <c r="C60" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>33</v>
       </c>
@@ -1484,8 +1526,9 @@
       <c r="C61" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>33</v>
       </c>
@@ -1495,8 +1538,9 @@
       <c r="C62" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>33</v>
       </c>
@@ -1506,8 +1550,9 @@
       <c r="C63" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>33</v>
       </c>
@@ -1517,8 +1562,9 @@
       <c r="C64" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>34</v>
       </c>
@@ -1528,8 +1574,9 @@
       <c r="C65" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>35</v>
       </c>
@@ -1539,8 +1586,9 @@
       <c r="C66" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>35</v>
       </c>
@@ -1550,8 +1598,9 @@
       <c r="C67" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>35</v>
       </c>
@@ -1561,8 +1610,9 @@
       <c r="C68" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>35</v>
       </c>
@@ -1572,8 +1622,9 @@
       <c r="C69" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>35</v>
       </c>
@@ -1583,8 +1634,9 @@
       <c r="C70" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>35</v>
       </c>
@@ -1594,8 +1646,9 @@
       <c r="C71" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>12</v>
       </c>
@@ -1605,8 +1658,9 @@
       <c r="C72" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>36</v>
       </c>
@@ -1616,8 +1670,9 @@
       <c r="C73" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>36</v>
       </c>
@@ -1627,8 +1682,9 @@
       <c r="C74" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>36</v>
       </c>
@@ -1638,8 +1694,9 @@
       <c r="C75" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>36</v>
       </c>
@@ -1649,8 +1706,9 @@
       <c r="C76" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>36</v>
       </c>
@@ -1660,8 +1718,9 @@
       <c r="C77" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>37</v>
       </c>
@@ -1671,8 +1730,9 @@
       <c r="C78" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>37</v>
       </c>
@@ -1682,8 +1742,9 @@
       <c r="C79" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>38</v>
       </c>
@@ -1693,8 +1754,9 @@
       <c r="C80" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>38</v>
       </c>
@@ -1704,8 +1766,9 @@
       <c r="C81" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>38</v>
       </c>
@@ -1715,8 +1778,9 @@
       <c r="C82" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>9</v>
       </c>
@@ -1726,8 +1790,9 @@
       <c r="C83" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>9</v>
       </c>
@@ -1737,8 +1802,9 @@
       <c r="C84" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>9</v>
       </c>
@@ -1748,8 +1814,9 @@
       <c r="C85" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>2</v>
       </c>
@@ -1759,8 +1826,9 @@
       <c r="C86" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>2</v>
       </c>
@@ -1770,8 +1838,9 @@
       <c r="C87" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>4</v>
       </c>
@@ -1781,8 +1850,9 @@
       <c r="C88" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>4</v>
       </c>
@@ -1792,8 +1862,9 @@
       <c r="C89" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>11</v>
       </c>
@@ -1803,8 +1874,9 @@
       <c r="C90" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>39</v>
       </c>
@@ -1814,8 +1886,9 @@
       <c r="C91" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>40</v>
       </c>
@@ -1825,8 +1898,9 @@
       <c r="C92" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>40</v>
       </c>
@@ -1836,8 +1910,9 @@
       <c r="C93" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>40</v>
       </c>
@@ -1847,8 +1922,9 @@
       <c r="C94" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>41</v>
       </c>
@@ -1858,8 +1934,9 @@
       <c r="C95" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>41</v>
       </c>
@@ -1869,8 +1946,9 @@
       <c r="C96" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>41</v>
       </c>
@@ -1880,8 +1958,9 @@
       <c r="C97" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>1</v>
       </c>
@@ -1891,8 +1970,9 @@
       <c r="C98" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>10</v>
       </c>
@@ -1902,8 +1982,9 @@
       <c r="C99" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>10</v>
       </c>
@@ -1913,8 +1994,9 @@
       <c r="C100" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>42</v>
       </c>
@@ -1924,8 +2006,9 @@
       <c r="C101" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>43</v>
       </c>
@@ -1935,8 +2018,9 @@
       <c r="C102" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>44</v>
       </c>
@@ -1946,8 +2030,9 @@
       <c r="C103" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>45</v>
       </c>
@@ -1957,8 +2042,9 @@
       <c r="C104" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>46</v>
       </c>
@@ -1968,8 +2054,9 @@
       <c r="C105" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>47</v>
       </c>
@@ -1979,8 +2066,9 @@
       <c r="C106" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>48</v>
       </c>
@@ -1990,8 +2078,9 @@
       <c r="C107" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>49</v>
       </c>
@@ -2001,8 +2090,9 @@
       <c r="C108" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>50</v>
       </c>
@@ -2012,8 +2102,9 @@
       <c r="C109" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>51</v>
       </c>
@@ -2023,8 +2114,9 @@
       <c r="C110" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>52</v>
       </c>
@@ -2034,8 +2126,9 @@
       <c r="C111" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>53</v>
       </c>
@@ -2045,8 +2138,9 @@
       <c r="C112" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>54</v>
       </c>
@@ -2056,8 +2150,9 @@
       <c r="C113" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>55</v>
       </c>
@@ -2067,8 +2162,9 @@
       <c r="C114" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>56</v>
       </c>
@@ -2078,8 +2174,9 @@
       <c r="C115" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>57</v>
       </c>
@@ -2089,8 +2186,9 @@
       <c r="C116" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>58</v>
       </c>
@@ -2100,8 +2198,9 @@
       <c r="C117" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>59</v>
       </c>
@@ -2111,8 +2210,9 @@
       <c r="C118" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>60</v>
       </c>
@@ -2122,8 +2222,9 @@
       <c r="C119" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>61</v>
       </c>
@@ -2133,8 +2234,9 @@
       <c r="C120" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>62</v>
       </c>
@@ -2144,8 +2246,9 @@
       <c r="C121" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D121"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>63</v>
       </c>
@@ -2155,8 +2258,9 @@
       <c r="C122" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D122"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>64</v>
       </c>
@@ -2166,8 +2270,9 @@
       <c r="C123" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>65</v>
       </c>
@@ -2177,8 +2282,9 @@
       <c r="C124" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D124"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>66</v>
       </c>
@@ -2188,8 +2294,9 @@
       <c r="C125" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>67</v>
       </c>
@@ -2199,8 +2306,9 @@
       <c r="C126" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D126"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>68</v>
       </c>
@@ -2210,8 +2318,9 @@
       <c r="C127" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D127"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>69</v>
       </c>
@@ -2221,8 +2330,9 @@
       <c r="C128" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D128"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>70</v>
       </c>
@@ -2232,8 +2342,9 @@
       <c r="C129" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D129"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>71</v>
       </c>
@@ -2243,8 +2354,9 @@
       <c r="C130" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D130"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>72</v>
       </c>
@@ -2254,8 +2366,9 @@
       <c r="C131" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D131"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>73</v>
       </c>
@@ -2265,8 +2378,9 @@
       <c r="C132" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D132"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>74</v>
       </c>
@@ -2276,8 +2390,9 @@
       <c r="C133" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D133"/>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>75</v>
       </c>
@@ -2287,8 +2402,9 @@
       <c r="C134" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D134"/>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>76</v>
       </c>
@@ -2298,8 +2414,9 @@
       <c r="C135" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D135"/>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>77</v>
       </c>
@@ -2309,8 +2426,10 @@
       <c r="C136" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D136"/>
+      <c r="H136"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>78</v>
       </c>
@@ -2320,8 +2439,10 @@
       <c r="C137" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D137"/>
+      <c r="H137"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>79</v>
       </c>
@@ -2331,8 +2452,10 @@
       <c r="C138" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D138"/>
+      <c r="H138"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>80</v>
       </c>
@@ -2342,8 +2465,10 @@
       <c r="C139" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D139"/>
+      <c r="H139"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>81</v>
       </c>
@@ -2353,8 +2478,10 @@
       <c r="C140" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D140"/>
+      <c r="H140"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>82</v>
       </c>
@@ -2364,8 +2491,10 @@
       <c r="C141" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D141"/>
+      <c r="H141"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>83</v>
       </c>
@@ -2375,8 +2504,10 @@
       <c r="C142" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D142"/>
+      <c r="H142"/>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>84</v>
       </c>
@@ -2386,8 +2517,10 @@
       <c r="C143" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D143"/>
+      <c r="H143"/>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>85</v>
       </c>
@@ -2397,8 +2530,10 @@
       <c r="C144" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D144"/>
+      <c r="H144"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>86</v>
       </c>
@@ -2408,8 +2543,10 @@
       <c r="C145" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D145"/>
+      <c r="H145"/>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>87</v>
       </c>
@@ -2419,8 +2556,10 @@
       <c r="C146" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D146"/>
+      <c r="H146"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>88</v>
       </c>
@@ -2430,8 +2569,10 @@
       <c r="C147" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D147"/>
+      <c r="H147"/>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>89</v>
       </c>
@@ -2441,8 +2582,10 @@
       <c r="C148" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D148"/>
+      <c r="H148"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>90</v>
       </c>
@@ -2452,8 +2595,10 @@
       <c r="C149" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D149"/>
+      <c r="H149"/>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>91</v>
       </c>
@@ -2463,8 +2608,10 @@
       <c r="C150" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D150"/>
+      <c r="H150"/>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>92</v>
       </c>
@@ -2474,8 +2621,10 @@
       <c r="C151" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D151"/>
+      <c r="H151"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>93</v>
       </c>
@@ -2485,8 +2634,10 @@
       <c r="C152" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D152"/>
+      <c r="H152"/>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>94</v>
       </c>
@@ -2496,8 +2647,10 @@
       <c r="C153" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D153"/>
+      <c r="H153"/>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>95</v>
       </c>
@@ -2507,8 +2660,10 @@
       <c r="C154" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D154"/>
+      <c r="H154"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>96</v>
       </c>
@@ -2518,8 +2673,10 @@
       <c r="C155" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D155"/>
+      <c r="H155"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>97</v>
       </c>
@@ -2529,8 +2686,10 @@
       <c r="C156" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D156"/>
+      <c r="H156"/>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>98</v>
       </c>
@@ -2540,8 +2699,10 @@
       <c r="C157" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D157"/>
+      <c r="H157"/>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>99</v>
       </c>
@@ -2551,8 +2712,10 @@
       <c r="C158" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D158"/>
+      <c r="H158"/>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>100</v>
       </c>
@@ -2562,8 +2725,10 @@
       <c r="C159" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D159"/>
+      <c r="H159"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>101</v>
       </c>
@@ -2573,8 +2738,10 @@
       <c r="C160" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D160"/>
+      <c r="H160"/>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>102</v>
       </c>
@@ -2584,8 +2751,10 @@
       <c r="C161" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D161"/>
+      <c r="H161"/>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>103</v>
       </c>
@@ -2595,8 +2764,10 @@
       <c r="C162" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D162"/>
+      <c r="H162"/>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>104</v>
       </c>
@@ -2606,8 +2777,10 @@
       <c r="C163" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D163"/>
+      <c r="H163"/>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>105</v>
       </c>
@@ -2617,8 +2790,10 @@
       <c r="C164" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D164"/>
+      <c r="H164"/>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>106</v>
       </c>
@@ -2628,8 +2803,10 @@
       <c r="C165" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D165"/>
+      <c r="H165"/>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>107</v>
       </c>
@@ -2639,8 +2816,10 @@
       <c r="C166" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D166"/>
+      <c r="H166"/>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>108</v>
       </c>
@@ -2650,8 +2829,10 @@
       <c r="C167" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D167"/>
+      <c r="H167"/>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>109</v>
       </c>
@@ -2661,8 +2842,10 @@
       <c r="C168" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D168"/>
+      <c r="H168"/>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>110</v>
       </c>
@@ -2672,8 +2855,10 @@
       <c r="C169" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D169"/>
+      <c r="H169"/>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>111</v>
       </c>
@@ -2683,8 +2868,10 @@
       <c r="C170" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D170"/>
+      <c r="H170"/>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>112</v>
       </c>
@@ -2694,8 +2881,10 @@
       <c r="C171" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D171"/>
+      <c r="H171"/>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>113</v>
       </c>
@@ -2705,8 +2894,10 @@
       <c r="C172" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D172"/>
+      <c r="H172"/>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>114</v>
       </c>
@@ -2716,8 +2907,10 @@
       <c r="C173" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D173"/>
+      <c r="H173"/>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>115</v>
       </c>
@@ -2727,8 +2920,10 @@
       <c r="C174" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D174"/>
+      <c r="H174"/>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>116</v>
       </c>
@@ -2738,8 +2933,10 @@
       <c r="C175" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D175"/>
+      <c r="H175"/>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>117</v>
       </c>
@@ -2749,8 +2946,10 @@
       <c r="C176" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D176"/>
+      <c r="H176"/>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>118</v>
       </c>
@@ -2760,8 +2959,10 @@
       <c r="C177" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D177"/>
+      <c r="H177"/>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>119</v>
       </c>
@@ -2771,8 +2972,10 @@
       <c r="C178" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D178"/>
+      <c r="H178"/>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>120</v>
       </c>
@@ -2782,8 +2985,10 @@
       <c r="C179" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D179"/>
+      <c r="H179"/>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>121</v>
       </c>
@@ -2793,8 +2998,10 @@
       <c r="C180" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D180"/>
+      <c r="H180"/>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>122</v>
       </c>
@@ -2804,8 +3011,10 @@
       <c r="C181" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D181"/>
+      <c r="H181"/>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>123</v>
       </c>
@@ -2815,8 +3024,10 @@
       <c r="C182" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D182"/>
+      <c r="H182"/>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>124</v>
       </c>
@@ -2826,8 +3037,10 @@
       <c r="C183" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D183"/>
+      <c r="H183"/>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>125</v>
       </c>
@@ -2837,8 +3050,10 @@
       <c r="C184" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D184"/>
+      <c r="H184"/>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>126</v>
       </c>
@@ -2848,8 +3063,10 @@
       <c r="C185" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D185"/>
+      <c r="H185"/>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>127</v>
       </c>
@@ -2859,8 +3076,10 @@
       <c r="C186" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D186"/>
+      <c r="H186"/>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>128</v>
       </c>
@@ -2870,8 +3089,10 @@
       <c r="C187" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D187"/>
+      <c r="H187"/>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>129</v>
       </c>
@@ -2881,8 +3102,10 @@
       <c r="C188" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D188"/>
+      <c r="H188"/>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>130</v>
       </c>
@@ -2892,8 +3115,10 @@
       <c r="C189" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D189"/>
+      <c r="H189"/>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>131</v>
       </c>
@@ -2903,8 +3128,10 @@
       <c r="C190" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D190"/>
+      <c r="H190"/>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>132</v>
       </c>
@@ -2914,8 +3141,10 @@
       <c r="C191" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D191"/>
+      <c r="H191"/>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>133</v>
       </c>
@@ -2925,8 +3154,10 @@
       <c r="C192" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D192"/>
+      <c r="H192"/>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>134</v>
       </c>
@@ -2936,8 +3167,10 @@
       <c r="C193" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D193"/>
+      <c r="H193"/>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>135</v>
       </c>
@@ -2947,47 +3180,49 @@
       <c r="C194" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D194"/>
+      <c r="H194"/>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B195" s="3"/>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B196" s="3"/>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B197" s="3"/>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B198" s="3"/>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B199" s="3"/>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B200" s="3"/>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B201" s="3"/>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B202" s="3"/>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B203" s="3"/>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B204" s="3"/>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B205" s="3"/>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B206" s="3"/>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B207" s="3"/>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B208" s="3"/>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Change derivation methods adding a flag to allow (or not) derivation of original tons. Optimization strategies now call derivation methods not allowing original tons to be derived.
</commit_message>
<xml_diff>
--- a/data/railway_od_pairs.xlsx
+++ b/data/railway_od_pairs.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$B$2458</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$189</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="136">
   <si>
     <t>30-45</t>
   </si>
@@ -274,12 +274,6 @@
     <t>3-26</t>
   </si>
   <si>
-    <t>1-1021</t>
-  </si>
-  <si>
-    <t>21-1021</t>
-  </si>
-  <si>
     <t>1022-1052</t>
   </si>
   <si>
@@ -394,12 +388,6 @@
     <t>19-43</t>
   </si>
   <si>
-    <t>55-64</t>
-  </si>
-  <si>
-    <t>55-56</t>
-  </si>
-  <si>
     <t>68-79</t>
   </si>
   <si>
@@ -428,6 +416,15 @@
   </si>
   <si>
     <t>railway_category</t>
+  </si>
+  <si>
+    <t>29-36</t>
+  </si>
+  <si>
+    <t>1-21</t>
+  </si>
+  <si>
+    <t>56-64</t>
   </si>
 </sst>
 </file>
@@ -782,7 +779,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5304"/>
+  <dimension ref="A1:H5299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -793,7 +790,8 @@
     <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -804,88 +802,88 @@
         <v>15</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3">
-        <v>127540.52073273997</v>
+        <v>1760200</v>
       </c>
       <c r="C2" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="B3" s="3">
-        <v>29141.286038496473</v>
+        <v>1056188</v>
       </c>
       <c r="C3" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3">
-        <v>37816</v>
+        <v>747500</v>
       </c>
       <c r="C4" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B5" s="3">
-        <v>35481.353006894577</v>
+        <v>547800</v>
       </c>
       <c r="C5" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3">
-        <v>9068.9813571231753</v>
+        <v>544966.78</v>
       </c>
       <c r="C6" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3">
-        <v>66178</v>
+        <v>525676.78</v>
       </c>
       <c r="C7" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3">
-        <v>33217.576403841915</v>
+        <v>522320.76434067497</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -894,22 +892,22 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B9" s="3">
-        <v>13119.245591411502</v>
+        <v>471153.64</v>
       </c>
       <c r="C9" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B10" s="3">
-        <v>93185.75</v>
+        <v>469086.70666041004</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -918,46 +916,46 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="B11" s="3">
-        <v>37343.200000000004</v>
+        <v>443300</v>
       </c>
       <c r="C11" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3">
-        <v>42403.198614379697</v>
+        <v>420390.21</v>
       </c>
       <c r="C12" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D12"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="B13" s="3">
-        <v>29281.503377839501</v>
+        <v>417600</v>
       </c>
       <c r="C13" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B14" s="3">
-        <v>65350.6</v>
+        <v>415671.11832148652</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
@@ -966,10 +964,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B15" s="3">
-        <v>68801.596510717645</v>
+        <v>410144.22725310811</v>
       </c>
       <c r="C15" s="4">
         <v>1</v>
@@ -978,10 +976,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B16" s="3">
-        <v>99894.503913999608</v>
+        <v>397017.5</v>
       </c>
       <c r="C16" s="4">
         <v>1</v>
@@ -990,22 +988,22 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B17" s="3">
-        <v>65936.829161201429</v>
+        <v>379269.4</v>
       </c>
       <c r="C17" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D17"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3">
-        <v>212671.9</v>
+        <v>378193.7991551407</v>
       </c>
       <c r="C18" s="4">
         <v>1</v>
@@ -1014,22 +1012,22 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="B19" s="3">
-        <v>67508.67747857995</v>
+        <v>369953.46</v>
       </c>
       <c r="C19" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D19"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B20" s="3">
-        <v>213188.01872256826</v>
+        <v>353002.61416723503</v>
       </c>
       <c r="C20" s="4">
         <v>1</v>
@@ -1038,10 +1036,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B21" s="3">
-        <v>55978.568292450909</v>
+        <v>335584.52129543561</v>
       </c>
       <c r="C21" s="4">
         <v>1</v>
@@ -1050,10 +1048,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B22" s="3">
-        <v>71045.437236189377</v>
+        <v>317614</v>
       </c>
       <c r="C22" s="4">
         <v>1</v>
@@ -1062,10 +1060,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B23" s="3">
-        <v>44509.516262606776</v>
+        <v>292837.96762648539</v>
       </c>
       <c r="C23" s="4">
         <v>1</v>
@@ -1074,34 +1072,34 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="B24" s="3">
-        <v>191779.62637205271</v>
+        <v>277638.37</v>
       </c>
       <c r="C24" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D24"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="B25" s="3">
-        <v>258296.192952385</v>
+        <v>270832.71000000002</v>
       </c>
       <c r="C25" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D25"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B26" s="3">
-        <v>104890</v>
+        <v>268812.21523172566</v>
       </c>
       <c r="C26" s="4">
         <v>1</v>
@@ -1110,34 +1108,34 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="B27" s="3">
-        <v>152639.10532840685</v>
+        <v>266533.21999999997</v>
       </c>
       <c r="C27" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D27"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="B28" s="3">
-        <v>137858.63226857415</v>
+        <v>263200</v>
       </c>
       <c r="C28" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D28"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B29" s="3">
-        <v>47130.70440228939</v>
+        <v>258296.192952385</v>
       </c>
       <c r="C29" s="4">
         <v>1</v>
@@ -1146,10 +1144,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B30" s="3">
-        <v>201995.06655613636</v>
+        <v>244444.90868565158</v>
       </c>
       <c r="C30" s="4">
         <v>1</v>
@@ -1158,22 +1156,22 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="B31" s="3">
-        <v>144958.41277428553</v>
+        <v>240000</v>
       </c>
       <c r="C31" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D31"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B32" s="3">
-        <v>30420.800000000003</v>
+        <v>238969.13590303698</v>
       </c>
       <c r="C32" s="4">
         <v>1</v>
@@ -1182,10 +1180,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B33" s="3">
-        <v>20596.627243388237</v>
+        <v>234270.38837124861</v>
       </c>
       <c r="C33" s="4">
         <v>1</v>
@@ -1194,46 +1192,46 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="B34" s="3">
-        <v>41592.459680903834</v>
+        <v>227700</v>
       </c>
       <c r="C34" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D34"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="B35" s="3">
-        <v>53236.399999999994</v>
+        <v>225366.86</v>
       </c>
       <c r="C35" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D35"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B36" s="3">
-        <v>116682.87752585208</v>
+        <v>216467.29</v>
       </c>
       <c r="C36" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D36"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B37" s="3">
-        <v>205678.75</v>
+        <v>213188.01872256826</v>
       </c>
       <c r="C37" s="4">
         <v>1</v>
@@ -1242,10 +1240,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B38" s="3">
-        <v>112528.15499452136</v>
+        <v>212671.9</v>
       </c>
       <c r="C38" s="4">
         <v>1</v>
@@ -1254,10 +1252,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B39" s="3">
-        <v>72304</v>
+        <v>205678.75</v>
       </c>
       <c r="C39" s="4">
         <v>1</v>
@@ -1266,10 +1264,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="B40" s="3">
-        <v>83486.974537763585</v>
+        <v>201995.06655613636</v>
       </c>
       <c r="C40" s="4">
         <v>1</v>
@@ -1278,22 +1276,22 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B41" s="3">
-        <v>16826.122601439787</v>
+        <v>198197.5</v>
       </c>
       <c r="C41" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D41"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B42" s="3">
-        <v>90380</v>
+        <v>191991.54163750727</v>
       </c>
       <c r="C42" s="4">
         <v>1</v>
@@ -1302,10 +1300,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B43" s="3">
-        <v>173176.64013155986</v>
+        <v>191779.62637205271</v>
       </c>
       <c r="C43" s="4">
         <v>1</v>
@@ -1314,58 +1312,58 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="B44" s="3">
-        <v>95477.001351254483</v>
+        <v>190000</v>
       </c>
       <c r="C44" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D44"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="B45" s="3">
-        <v>124560.47698791185</v>
+        <v>185524.46</v>
       </c>
       <c r="C45" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D45"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="B46" s="3">
-        <v>152639.10532840685</v>
+        <v>181979.39</v>
       </c>
       <c r="C46" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D46"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="B47" s="3">
-        <v>146521.14947738417</v>
+        <v>176700.57</v>
       </c>
       <c r="C47" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D47"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B48" s="3">
-        <v>55781.748168259932</v>
+        <v>174709.43579285187</v>
       </c>
       <c r="C48" s="4">
         <v>1</v>
@@ -1374,10 +1372,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B49" s="3">
-        <v>39612.484515818447</v>
+        <v>173176.64013155986</v>
       </c>
       <c r="C49" s="4">
         <v>1</v>
@@ -1386,25 +1384,25 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="B50" s="3">
-        <v>132928.49140242304</v>
+        <v>170000</v>
       </c>
       <c r="C50" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D50"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="B51" s="3">
-        <v>17537.295581713413</v>
+        <v>163224.34</v>
       </c>
       <c r="C51" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D51"/>
     </row>
@@ -1413,7 +1411,7 @@
         <v>30</v>
       </c>
       <c r="B52" s="3">
-        <v>35762.163434948634</v>
+        <v>153087.23278307472</v>
       </c>
       <c r="C52" s="4">
         <v>1</v>
@@ -1422,10 +1420,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
       <c r="B53" s="3">
-        <v>153087.23278307472</v>
+        <v>152639.10532840685</v>
       </c>
       <c r="C53" s="4">
         <v>1</v>
@@ -1434,34 +1432,34 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="B54" s="3">
-        <v>35762.163434948663</v>
+        <v>150000</v>
       </c>
       <c r="C54" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D54"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B55" s="3">
-        <v>410144.22725310811</v>
+        <v>147184.04999999999</v>
       </c>
       <c r="C55" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D55"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B56" s="3">
-        <v>238969.13590303698</v>
+        <v>146521.14947738417</v>
       </c>
       <c r="C56" s="4">
         <v>1</v>
@@ -1470,10 +1468,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="B57" s="3">
-        <v>32586</v>
+        <v>144958.41277428553</v>
       </c>
       <c r="C57" s="4">
         <v>1</v>
@@ -1482,10 +1480,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="B58" s="3">
-        <v>101400.90158853697</v>
+        <v>142862.46877182633</v>
       </c>
       <c r="C58" s="4">
         <v>1</v>
@@ -1494,10 +1492,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B59" s="3">
-        <v>48615.600000000006</v>
+        <v>139761.87565104209</v>
       </c>
       <c r="C59" s="4">
         <v>1</v>
@@ -1506,10 +1504,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="B60" s="3">
-        <v>234270.38837124861</v>
+        <v>137858.63226857415</v>
       </c>
       <c r="C60" s="4">
         <v>1</v>
@@ -1518,10 +1516,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B61" s="3">
-        <v>244444.90868565158</v>
+        <v>132928.49140242304</v>
       </c>
       <c r="C61" s="4">
         <v>1</v>
@@ -1530,22 +1528,22 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="B62" s="3">
-        <v>26718.876238633235</v>
+        <v>132715.46</v>
       </c>
       <c r="C62" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D62"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B63" s="3">
-        <v>292837.96762648539</v>
+        <v>130197.86528291726</v>
       </c>
       <c r="C63" s="4">
         <v>1</v>
@@ -1554,10 +1552,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B64" s="3">
-        <v>79813.308256947086</v>
+        <v>127540.52073273997</v>
       </c>
       <c r="C64" s="4">
         <v>1</v>
@@ -1566,22 +1564,22 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="B65" s="3">
-        <v>16634.400000000001</v>
+        <v>125359.69</v>
       </c>
       <c r="C65" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D65"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B66" s="3">
-        <v>94968.612065456342</v>
+        <v>124560.47698791185</v>
       </c>
       <c r="C66" s="4">
         <v>1</v>
@@ -1590,10 +1588,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="B67" s="3">
-        <v>335584.52129543561</v>
+        <v>118853.04204314978</v>
       </c>
       <c r="C67" s="4">
         <v>1</v>
@@ -1605,7 +1603,7 @@
         <v>35</v>
       </c>
       <c r="B68" s="3">
-        <v>58754.554557901625</v>
+        <v>118710.76508182043</v>
       </c>
       <c r="C68" s="4">
         <v>1</v>
@@ -1614,10 +1612,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B69" s="3">
-        <v>415671.11832148652</v>
+        <v>116682.87752585208</v>
       </c>
       <c r="C69" s="4">
         <v>1</v>
@@ -1626,10 +1624,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B70" s="3">
-        <v>71279.044416608842</v>
+        <v>112528.15499452136</v>
       </c>
       <c r="C70" s="4">
         <v>1</v>
@@ -1638,10 +1636,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B71" s="3">
-        <v>118710.76508182043</v>
+        <v>104890</v>
       </c>
       <c r="C71" s="4">
         <v>1</v>
@@ -1650,13 +1648,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="B72" s="3">
-        <v>15928.499999999998</v>
+        <v>104500</v>
       </c>
       <c r="C72" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D72"/>
     </row>
@@ -1665,7 +1663,7 @@
         <v>36</v>
       </c>
       <c r="B73" s="3">
-        <v>21436.052816368221</v>
+        <v>104275.06542306861</v>
       </c>
       <c r="C73" s="4">
         <v>1</v>
@@ -1674,10 +1672,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B74" s="3">
-        <v>45612.352414952475</v>
+        <v>101400.90158853697</v>
       </c>
       <c r="C74" s="4">
         <v>1</v>
@@ -1686,34 +1684,34 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="B75" s="3">
-        <v>522320.76434067497</v>
+        <v>100465.79</v>
       </c>
       <c r="C75" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D75"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="B76" s="3">
-        <v>104275.06542306861</v>
+        <v>100000</v>
       </c>
       <c r="C76" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D76"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B77" s="3">
-        <v>21436.052816368232</v>
+        <v>99894.503913999608</v>
       </c>
       <c r="C77" s="4">
         <v>1</v>
@@ -1722,22 +1720,22 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="B78" s="3">
-        <v>19508</v>
+        <v>96800</v>
       </c>
       <c r="C78" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D78"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="B79" s="3">
-        <v>19508</v>
+        <v>95477.001351254483</v>
       </c>
       <c r="C79" s="4">
         <v>1</v>
@@ -1746,10 +1744,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B80" s="3">
-        <v>130197.86528291726</v>
+        <v>94968.612065456342</v>
       </c>
       <c r="C80" s="4">
         <v>1</v>
@@ -1758,10 +1756,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B81" s="3">
-        <v>14262.918822015883</v>
+        <v>93185.75</v>
       </c>
       <c r="C81" s="4">
         <v>1</v>
@@ -1770,22 +1768,22 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="B82" s="3">
-        <v>268812.21523172566</v>
+        <v>90523.971999999994</v>
       </c>
       <c r="C82" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D82"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B83" s="3">
-        <v>317614</v>
+        <v>90380</v>
       </c>
       <c r="C83" s="4">
         <v>1</v>
@@ -1794,22 +1792,22 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B84" s="3">
-        <v>353002.61416723503</v>
+        <v>87500</v>
       </c>
       <c r="C84" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D84"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B85" s="3">
-        <v>397017.5</v>
+        <v>83486.974537763585</v>
       </c>
       <c r="C85" s="4">
         <v>1</v>
@@ -1818,10 +1816,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="B86" s="3">
-        <v>118853.04204314978</v>
+        <v>82724.929167692113</v>
       </c>
       <c r="C86" s="4">
         <v>1</v>
@@ -1830,22 +1828,22 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="B87" s="3">
-        <v>18062.983557381482</v>
+        <v>81794.334000000003</v>
       </c>
       <c r="C87" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D87"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B88" s="3">
-        <v>142862.46877182633</v>
+        <v>79813.308256947086</v>
       </c>
       <c r="C88" s="4">
         <v>1</v>
@@ -1854,82 +1852,82 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B89" s="3">
+        <v>77500</v>
+      </c>
+      <c r="C89" s="4">
         <v>4</v>
-      </c>
-      <c r="B89" s="3">
-        <v>74716.635230199157</v>
-      </c>
-      <c r="C89" s="4">
-        <v>1</v>
       </c>
       <c r="D89"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="B90" s="3">
-        <v>174709.43579285187</v>
+        <v>77011.194000000003</v>
       </c>
       <c r="C90" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D90"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="B91" s="3">
-        <v>139761.87565104209</v>
+        <v>77010</v>
       </c>
       <c r="C91" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D91"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="B92" s="3">
-        <v>469086.70666041004</v>
+        <v>75118.187000000005</v>
       </c>
       <c r="C92" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D92"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="B93" s="3">
-        <v>82724.929167692113</v>
+        <v>75016</v>
       </c>
       <c r="C93" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D93"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>40</v>
+        <v>134</v>
       </c>
       <c r="B94" s="3">
-        <v>191991.54163750727</v>
+        <v>75000</v>
       </c>
       <c r="C94" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D94"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="B95" s="3">
-        <v>37088.48457993153</v>
+        <v>74716.635230199157</v>
       </c>
       <c r="C95" s="4">
         <v>1</v>
@@ -1938,10 +1936,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B96" s="3">
-        <v>3367.7219768398677</v>
+        <v>72304</v>
       </c>
       <c r="C96" s="4">
         <v>1</v>
@@ -1950,10 +1948,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B97" s="3">
-        <v>37088.484579931552</v>
+        <v>71279.044416608842</v>
       </c>
       <c r="C97" s="4">
         <v>1</v>
@@ -1962,10 +1960,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B98" s="3">
-        <v>5849.0172573820937</v>
+        <v>71045.437236189377</v>
       </c>
       <c r="C98" s="4">
         <v>1</v>
@@ -1974,10 +1972,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B99" s="3">
-        <v>378193.7991551407</v>
+        <v>68801.596510717645</v>
       </c>
       <c r="C99" s="4">
         <v>1</v>
@@ -1986,10 +1984,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B100" s="3">
-        <v>41430.383244903285</v>
+        <v>67508.67747857995</v>
       </c>
       <c r="C100" s="4">
         <v>1</v>
@@ -1998,10 +1996,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="B101" s="3">
-        <v>1760200</v>
+        <v>66520.254000000001</v>
       </c>
       <c r="C101" s="4">
         <v>4</v>
@@ -2010,46 +2008,46 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B102" s="3">
-        <v>1056188</v>
+        <v>66178</v>
       </c>
       <c r="C102" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D102"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B103" s="3">
-        <v>747500</v>
+        <v>65936.829161201429</v>
       </c>
       <c r="C103" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D103"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="B104" s="3">
-        <v>547800</v>
+        <v>65350.6</v>
       </c>
       <c r="C104" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D104"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="B105" s="3">
-        <v>544966.78</v>
+        <v>63500</v>
       </c>
       <c r="C105" s="4">
         <v>4</v>
@@ -2058,10 +2056,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="B106" s="3">
-        <v>525676.78</v>
+        <v>62500</v>
       </c>
       <c r="C106" s="4">
         <v>4</v>
@@ -2070,10 +2068,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="B107" s="3">
-        <v>471153.64</v>
+        <v>62142.519</v>
       </c>
       <c r="C107" s="4">
         <v>4</v>
@@ -2082,10 +2080,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="B108" s="3">
-        <v>443300</v>
+        <v>60366.972000000002</v>
       </c>
       <c r="C108" s="4">
         <v>4</v>
@@ -2094,22 +2092,22 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B109" s="3">
-        <v>420390.21</v>
+        <v>58754.554557901625</v>
       </c>
       <c r="C109" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D109"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="B110" s="3">
-        <v>417600</v>
+        <v>58044.334000000003</v>
       </c>
       <c r="C110" s="4">
         <v>4</v>
@@ -2118,10 +2116,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="B111" s="3">
-        <v>379269.4</v>
+        <v>57250</v>
       </c>
       <c r="C111" s="4">
         <v>4</v>
@@ -2130,10 +2128,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="B112" s="3">
-        <v>369953.46</v>
+        <v>57200</v>
       </c>
       <c r="C112" s="4">
         <v>4</v>
@@ -2142,10 +2140,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="B113" s="3">
-        <v>277638.37</v>
+        <v>56100</v>
       </c>
       <c r="C113" s="4">
         <v>4</v>
@@ -2154,10 +2152,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="B114" s="3">
-        <v>270832.71000000002</v>
+        <v>56100</v>
       </c>
       <c r="C114" s="4">
         <v>4</v>
@@ -2166,46 +2164,46 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="B115" s="3">
-        <v>266533.21999999997</v>
+        <v>55978.568292450909</v>
       </c>
       <c r="C115" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D115"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="B116" s="3">
-        <v>263200</v>
+        <v>55781.748168259932</v>
       </c>
       <c r="C116" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D116"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="B117" s="3">
-        <v>240000</v>
+        <v>53236.399999999994</v>
       </c>
       <c r="C117" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D117"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="B118" s="3">
-        <v>227700</v>
+        <v>52187.514999999999</v>
       </c>
       <c r="C118" s="4">
         <v>4</v>
@@ -2214,10 +2212,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="B119" s="3">
-        <v>225366.86</v>
+        <v>52000</v>
       </c>
       <c r="C119" s="4">
         <v>4</v>
@@ -2226,10 +2224,10 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="B120" s="3">
-        <v>216467.29</v>
+        <v>49975.902000000002</v>
       </c>
       <c r="C120" s="4">
         <v>4</v>
@@ -2238,10 +2236,10 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="B121" s="3">
-        <v>198197.5</v>
+        <v>49000</v>
       </c>
       <c r="C121" s="4">
         <v>4</v>
@@ -2250,22 +2248,22 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="B122" s="3">
-        <v>190000</v>
+        <v>48615.600000000006</v>
       </c>
       <c r="C122" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D122"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="B123" s="3">
-        <v>185524.46</v>
+        <v>47284.544000000002</v>
       </c>
       <c r="C123" s="4">
         <v>4</v>
@@ -2274,22 +2272,22 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="B124" s="3">
-        <v>181979.39</v>
+        <v>47130.70440228939</v>
       </c>
       <c r="C124" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D124"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="B125" s="3">
-        <v>176700.57</v>
+        <v>46485.449000000001</v>
       </c>
       <c r="C125" s="4">
         <v>4</v>
@@ -2298,22 +2296,22 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="B126" s="3">
-        <v>170000</v>
+        <v>45612.352414952475</v>
       </c>
       <c r="C126" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D126"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="B127" s="3">
-        <v>163224.34</v>
+        <v>45068.192999999999</v>
       </c>
       <c r="C127" s="4">
         <v>4</v>
@@ -2322,22 +2320,22 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="B128" s="3">
-        <v>150000</v>
+        <v>44509.516262606776</v>
       </c>
       <c r="C128" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D128"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="B129" s="3">
-        <v>147184.04999999999</v>
+        <v>43710.050999999999</v>
       </c>
       <c r="C129" s="4">
         <v>4</v>
@@ -2346,22 +2344,22 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="B130" s="3">
-        <v>132715.46</v>
+        <v>42403.198614379697</v>
       </c>
       <c r="C130" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D130"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="B131" s="3">
-        <v>125359.69</v>
+        <v>42133.027999999998</v>
       </c>
       <c r="C131" s="4">
         <v>4</v>
@@ -2370,58 +2368,60 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="B132" s="3">
-        <v>104500</v>
+        <v>41592.459680903834</v>
       </c>
       <c r="C132" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D132"/>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="B133" s="3">
-        <v>100465.79</v>
+        <v>41430.383244903285</v>
       </c>
       <c r="C133" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D133"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="B134" s="3">
-        <v>100000</v>
+        <v>41000</v>
       </c>
       <c r="C134" s="4">
         <v>4</v>
       </c>
       <c r="D134"/>
+      <c r="H134"/>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="B135" s="3">
-        <v>96800</v>
+        <v>39612.484515818447</v>
       </c>
       <c r="C135" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D135"/>
+      <c r="H135"/>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="B136" s="3">
-        <v>90523.971999999994</v>
+        <v>39490</v>
       </c>
       <c r="C136" s="4">
         <v>4</v>
@@ -2431,62 +2431,62 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="B137" s="3">
-        <v>87500</v>
+        <v>37816</v>
       </c>
       <c r="C137" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D137"/>
       <c r="H137"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="B138" s="3">
-        <v>81794.334000000003</v>
+        <v>37343.200000000004</v>
       </c>
       <c r="C138" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D138"/>
       <c r="H138"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="B139" s="3">
-        <v>77500</v>
+        <v>37088.484579931552</v>
       </c>
       <c r="C139" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D139"/>
       <c r="H139"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="B140" s="3">
-        <v>77011.194000000003</v>
+        <v>37088.48457993153</v>
       </c>
       <c r="C140" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D140"/>
       <c r="H140"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="B141" s="3">
-        <v>77010</v>
+        <v>36500</v>
       </c>
       <c r="C141" s="4">
         <v>4</v>
@@ -2496,10 +2496,10 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="B142" s="3">
-        <v>75118.187000000005</v>
+        <v>36261.805999999997</v>
       </c>
       <c r="C142" s="4">
         <v>4</v>
@@ -2509,10 +2509,10 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="B143" s="3">
-        <v>75016</v>
+        <v>36000</v>
       </c>
       <c r="C143" s="4">
         <v>4</v>
@@ -2522,36 +2522,36 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="B144" s="3">
-        <v>75000</v>
+        <v>35762.163434948663</v>
       </c>
       <c r="C144" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D144"/>
       <c r="H144"/>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="B145" s="3">
-        <v>75000</v>
+        <v>35762.163434948634</v>
       </c>
       <c r="C145" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D145"/>
       <c r="H145"/>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="B146" s="3">
-        <v>66520.254000000001</v>
+        <v>35500</v>
       </c>
       <c r="C146" s="4">
         <v>4</v>
@@ -2561,23 +2561,23 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="B147" s="3">
-        <v>63500</v>
+        <v>35481.353006894577</v>
       </c>
       <c r="C147" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D147"/>
       <c r="H147"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="B148" s="3">
-        <v>62500</v>
+        <v>34648.453999999998</v>
       </c>
       <c r="C148" s="4">
         <v>4</v>
@@ -2587,10 +2587,10 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="B149" s="3">
-        <v>62142.519</v>
+        <v>34100</v>
       </c>
       <c r="C149" s="4">
         <v>4</v>
@@ -2600,10 +2600,10 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="B150" s="3">
-        <v>60366.972000000002</v>
+        <v>33500</v>
       </c>
       <c r="C150" s="4">
         <v>4</v>
@@ -2613,36 +2613,36 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="B151" s="3">
-        <v>58044.334000000003</v>
+        <v>33217.576403841915</v>
       </c>
       <c r="C151" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D151"/>
       <c r="H151"/>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="B152" s="3">
-        <v>57250</v>
+        <v>32586</v>
       </c>
       <c r="C152" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D152"/>
       <c r="H152"/>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="B153" s="3">
-        <v>57200</v>
+        <v>31250</v>
       </c>
       <c r="C153" s="4">
         <v>4</v>
@@ -2652,23 +2652,23 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>95</v>
+        <v>13</v>
       </c>
       <c r="B154" s="3">
-        <v>56100</v>
+        <v>30420.800000000003</v>
       </c>
       <c r="C154" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D154"/>
       <c r="H154"/>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="B155" s="3">
-        <v>56100</v>
+        <v>30000</v>
       </c>
       <c r="C155" s="4">
         <v>4</v>
@@ -2678,49 +2678,49 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="B156" s="3">
-        <v>52187.514999999999</v>
+        <v>29281.503377839501</v>
       </c>
       <c r="C156" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D156"/>
       <c r="H156"/>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="B157" s="3">
-        <v>52000</v>
+        <v>29141.286038496473</v>
       </c>
       <c r="C157" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D157"/>
       <c r="H157"/>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>99</v>
+        <v>33</v>
       </c>
       <c r="B158" s="3">
-        <v>49975.902000000002</v>
+        <v>26718.876238633235</v>
       </c>
       <c r="C158" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D158"/>
       <c r="H158"/>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B159" s="3">
-        <v>49000</v>
+        <v>25300</v>
       </c>
       <c r="C159" s="4">
         <v>4</v>
@@ -2730,10 +2730,10 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="B160" s="3">
-        <v>47284.544000000002</v>
+        <v>22100</v>
       </c>
       <c r="C160" s="4">
         <v>4</v>
@@ -2743,23 +2743,23 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="B161" s="3">
-        <v>46485.449000000001</v>
+        <v>21436.052816368232</v>
       </c>
       <c r="C161" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D161"/>
       <c r="H161"/>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="B162" s="3">
-        <v>45068.192999999999</v>
+        <v>20900</v>
       </c>
       <c r="C162" s="4">
         <v>4</v>
@@ -2769,36 +2769,36 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>104</v>
+        <v>13</v>
       </c>
       <c r="B163" s="3">
-        <v>43710.050999999999</v>
+        <v>20596.627243388237</v>
       </c>
       <c r="C163" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D163"/>
       <c r="H163"/>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>105</v>
+        <v>37</v>
       </c>
       <c r="B164" s="3">
-        <v>42133.027999999998</v>
+        <v>19508</v>
       </c>
       <c r="C164" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D164"/>
       <c r="H164"/>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="B165" s="3">
-        <v>41000</v>
+        <v>18700</v>
       </c>
       <c r="C165" s="4">
         <v>4</v>
@@ -2808,49 +2808,49 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>107</v>
+        <v>2</v>
       </c>
       <c r="B166" s="3">
-        <v>39490</v>
+        <v>18062.983557381482</v>
       </c>
       <c r="C166" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D166"/>
       <c r="H166"/>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>108</v>
+        <v>3</v>
       </c>
       <c r="B167" s="3">
-        <v>36500</v>
+        <v>17537.295581713413</v>
       </c>
       <c r="C167" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D167"/>
       <c r="H167"/>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>109</v>
+        <v>28</v>
       </c>
       <c r="B168" s="3">
-        <v>36261.805999999997</v>
+        <v>16826.122601439787</v>
       </c>
       <c r="C168" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D168"/>
       <c r="H168"/>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B169" s="3">
-        <v>36000</v>
+        <v>16732.468000000001</v>
       </c>
       <c r="C169" s="4">
         <v>4</v>
@@ -2860,36 +2860,36 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>111</v>
+        <v>34</v>
       </c>
       <c r="B170" s="3">
-        <v>35500</v>
+        <v>16634.400000000001</v>
       </c>
       <c r="C170" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D170"/>
       <c r="H170"/>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="B171" s="3">
-        <v>34648.453999999998</v>
+        <v>15928.499999999998</v>
       </c>
       <c r="C171" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D171"/>
       <c r="H171"/>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B172" s="3">
-        <v>34100</v>
+        <v>14679.745999999999</v>
       </c>
       <c r="C172" s="4">
         <v>4</v>
@@ -2899,36 +2899,36 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>114</v>
+        <v>38</v>
       </c>
       <c r="B173" s="3">
-        <v>33500</v>
+        <v>14262.918822015883</v>
       </c>
       <c r="C173" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D173"/>
       <c r="H173"/>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>115</v>
+        <v>18</v>
       </c>
       <c r="B174" s="3">
-        <v>31250</v>
+        <v>13119.245591411502</v>
       </c>
       <c r="C174" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D174"/>
       <c r="H174"/>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B175" s="3">
-        <v>30000</v>
+        <v>13049.767</v>
       </c>
       <c r="C175" s="4">
         <v>4</v>
@@ -2938,10 +2938,10 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B176" s="3">
-        <v>25300</v>
+        <v>11914</v>
       </c>
       <c r="C176" s="4">
         <v>4</v>
@@ -2951,10 +2951,10 @@
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="B177" s="3">
-        <v>22100</v>
+        <v>11750</v>
       </c>
       <c r="C177" s="4">
         <v>4</v>
@@ -2964,10 +2964,10 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B178" s="3">
-        <v>20900</v>
+        <v>10955.665999999999</v>
       </c>
       <c r="C178" s="4">
         <v>4</v>
@@ -2977,10 +2977,10 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B179" s="3">
-        <v>18700</v>
+        <v>9500</v>
       </c>
       <c r="C179" s="4">
         <v>4</v>
@@ -2990,23 +2990,23 @@
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>121</v>
+        <v>17</v>
       </c>
       <c r="B180" s="3">
-        <v>16732.468000000001</v>
+        <v>9068.9813571231753</v>
       </c>
       <c r="C180" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D180"/>
       <c r="H180"/>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B181" s="3">
-        <v>14679.745999999999</v>
+        <v>8396.1929999999993</v>
       </c>
       <c r="C181" s="4">
         <v>4</v>
@@ -3016,23 +3016,23 @@
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="B182" s="3">
-        <v>13049.767</v>
+        <v>5849.0172573820937</v>
       </c>
       <c r="C182" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D182"/>
       <c r="H182"/>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B183" s="3">
-        <v>11914</v>
+        <v>5000</v>
       </c>
       <c r="C183" s="4">
         <v>4</v>
@@ -3042,10 +3042,10 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B184" s="3">
-        <v>11750</v>
+        <v>5000</v>
       </c>
       <c r="C184" s="4">
         <v>4</v>
@@ -3055,23 +3055,23 @@
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>126</v>
+        <v>41</v>
       </c>
       <c r="B185" s="3">
-        <v>11750</v>
+        <v>3367.7219768398677</v>
       </c>
       <c r="C185" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D185"/>
       <c r="H185"/>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B186" s="3">
-        <v>10955.665999999999</v>
+        <v>2500</v>
       </c>
       <c r="C186" s="4">
         <v>4</v>
@@ -3081,10 +3081,10 @@
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B187" s="3">
-        <v>9500</v>
+        <v>2167.2865000000002</v>
       </c>
       <c r="C187" s="4">
         <v>4</v>
@@ -3094,10 +3094,10 @@
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B188" s="3">
-        <v>8396.1929999999993</v>
+        <v>1000</v>
       </c>
       <c r="C188" s="4">
         <v>4</v>
@@ -3107,10 +3107,10 @@
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B189" s="3">
-        <v>5000</v>
+        <v>919.64323999999999</v>
       </c>
       <c r="C189" s="4">
         <v>4</v>
@@ -3119,110 +3119,60 @@
       <c r="H189"/>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A190" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B190" s="3">
-        <v>5000</v>
-      </c>
-      <c r="C190" s="4">
-        <v>4</v>
-      </c>
-      <c r="D190"/>
-      <c r="H190"/>
+      <c r="B190" s="3"/>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A191" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B191" s="3">
-        <v>2500</v>
-      </c>
-      <c r="C191" s="4">
-        <v>4</v>
-      </c>
-      <c r="D191"/>
-      <c r="H191"/>
+      <c r="B191" s="3"/>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A192" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B192" s="3">
-        <v>2167.2865000000002</v>
-      </c>
-      <c r="C192" s="4">
-        <v>4</v>
-      </c>
-      <c r="D192"/>
-      <c r="H192"/>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A193" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B193" s="3">
-        <v>1000</v>
-      </c>
-      <c r="C193" s="4">
-        <v>4</v>
-      </c>
-      <c r="D193"/>
-      <c r="H193"/>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A194" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B194" s="3">
-        <v>919.64323999999999</v>
-      </c>
-      <c r="C194" s="4">
-        <v>4</v>
-      </c>
-      <c r="D194"/>
-      <c r="H194"/>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B192" s="3"/>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B193" s="3"/>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B194" s="3"/>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B195" s="3"/>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B196" s="3"/>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B197" s="3"/>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B198" s="3"/>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B199" s="3"/>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B200" s="3"/>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B201" s="3"/>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B202" s="3"/>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B203" s="3"/>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B204" s="3"/>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B205" s="3"/>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B206" s="3"/>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B207" s="3"/>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B208" s="3"/>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.25">
@@ -18497,21 +18447,6 @@
     </row>
     <row r="5299" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5299" s="3"/>
-    </row>
-    <row r="5300" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5300" s="3"/>
-    </row>
-    <row r="5301" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5301" s="3"/>
-    </row>
-    <row r="5302" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5302" s="3"/>
-    </row>
-    <row r="5303" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5303" s="3"/>
-    </row>
-    <row r="5304" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5304" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes in parameters. Fix idle capacity of no regroup ods being written to links.
</commit_message>
<xml_diff>
--- a/data/railway_od_pairs.xlsx
+++ b/data/railway_od_pairs.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" iterate="1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="132">
   <si>
     <t>30-45</t>
   </si>
@@ -76,9 +76,6 @@
     <t>67-21</t>
   </si>
   <si>
-    <t>62-21</t>
-  </si>
-  <si>
     <t>49-45</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
   </si>
   <si>
     <t>56-21</t>
-  </si>
-  <si>
-    <t>72-21</t>
   </si>
   <si>
     <t>59-21</t>
@@ -416,51 +410,6 @@
   </si>
   <si>
     <t>tons</t>
-  </si>
-  <si>
-    <t>66-77</t>
-  </si>
-  <si>
-    <t>99-100</t>
-  </si>
-  <si>
-    <t>1-1021</t>
-  </si>
-  <si>
-    <t>96-97</t>
-  </si>
-  <si>
-    <t>91-92</t>
-  </si>
-  <si>
-    <t>38-39</t>
-  </si>
-  <si>
-    <t>36-1044</t>
-  </si>
-  <si>
-    <t>21-1021</t>
-  </si>
-  <si>
-    <t>17-18</t>
-  </si>
-  <si>
-    <t>78-1079</t>
-  </si>
-  <si>
-    <t>44-1044</t>
-  </si>
-  <si>
-    <t>35-1044</t>
-  </si>
-  <si>
-    <t>12-18</t>
-  </si>
-  <si>
-    <t>79-1079</t>
-  </si>
-  <si>
-    <t>22-1022</t>
   </si>
 </sst>
 </file>
@@ -816,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5297"/>
+  <dimension ref="A1:H5295"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="B189" sqref="B189"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A27" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,16 +785,16 @@
         <v>14</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3">
         <v>522320.76434067497</v>
@@ -857,7 +806,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="3">
         <v>469086.70666041004</v>
@@ -869,7 +818,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3">
         <v>415671.11832148652</v>
@@ -929,7 +878,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" s="3">
         <v>335584.52129543561</v>
@@ -953,7 +902,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3">
         <v>292837.96762648539</v>
@@ -965,7 +914,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" s="3">
         <v>268812.21523172566</v>
@@ -977,7 +926,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="3">
         <v>258296.192952385</v>
@@ -989,7 +938,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="3">
         <v>244444.90868565158</v>
@@ -1013,7 +962,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="3">
         <v>234270.38837124861</v>
@@ -1025,7 +974,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="3">
         <v>213188.01872256826</v>
@@ -1049,7 +998,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="3">
         <v>205678.75</v>
@@ -1073,7 +1022,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" s="3">
         <v>191991.54163750727</v>
@@ -1085,7 +1034,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3">
         <v>191779.62637205271</v>
@@ -1121,7 +1070,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25" s="3">
         <v>153087.23278307472</v>
@@ -1133,7 +1082,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B26" s="3">
         <v>152639.10532840685</v>
@@ -1181,7 +1130,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" s="3">
         <v>139761.87565104209</v>
@@ -1217,7 +1166,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B33" s="3">
         <v>130197.86528291726</v>
@@ -1265,7 +1214,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B37" s="3">
         <v>118710.76508182043</v>
@@ -1277,7 +1226,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B38" s="3">
         <v>116682.87752585208</v>
@@ -1289,10 +1238,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B39" s="3">
-        <v>112528.15499452136</v>
+        <v>104890</v>
       </c>
       <c r="C39" s="4">
         <v>1</v>
@@ -1301,10 +1250,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B40" s="3">
-        <v>104890</v>
+        <v>104275.06542306861</v>
       </c>
       <c r="C40" s="4">
         <v>1</v>
@@ -1313,10 +1262,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B41" s="3">
-        <v>104275.06542306861</v>
+        <v>101400.90158853697</v>
       </c>
       <c r="C41" s="4">
         <v>1</v>
@@ -1325,10 +1274,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B42" s="3">
-        <v>101400.90158853697</v>
+        <v>99894.503913999608</v>
       </c>
       <c r="C42" s="4">
         <v>1</v>
@@ -1337,10 +1286,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B43" s="3">
-        <v>99894.503913999608</v>
+        <v>95477.001351254483</v>
       </c>
       <c r="C43" s="4">
         <v>1</v>
@@ -1349,10 +1298,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B44" s="3">
-        <v>95477.001351254483</v>
+        <v>94968.612065456342</v>
       </c>
       <c r="C44" s="4">
         <v>1</v>
@@ -1361,10 +1310,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B45" s="3">
-        <v>94968.612065456342</v>
+        <v>93185.75</v>
       </c>
       <c r="C45" s="4">
         <v>1</v>
@@ -1373,10 +1322,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B46" s="3">
-        <v>93185.75</v>
+        <v>90380</v>
       </c>
       <c r="C46" s="4">
         <v>1</v>
@@ -1385,10 +1334,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B47" s="3">
-        <v>90380</v>
+        <v>83486.974537763585</v>
       </c>
       <c r="C47" s="4">
         <v>1</v>
@@ -1397,10 +1346,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B48" s="3">
-        <v>83486.974537763585</v>
+        <v>82724.929167692113</v>
       </c>
       <c r="C48" s="4">
         <v>1</v>
@@ -1409,10 +1358,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B49" s="3">
-        <v>82724.929167692113</v>
+        <v>79813.308256947086</v>
       </c>
       <c r="C49" s="4">
         <v>1</v>
@@ -1421,10 +1370,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="B50" s="3">
-        <v>79813.308256947086</v>
+        <v>74716.635230199157</v>
       </c>
       <c r="C50" s="4">
         <v>1</v>
@@ -1433,10 +1382,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B51" s="3">
-        <v>74716.635230199157</v>
+        <v>72304</v>
       </c>
       <c r="C51" s="4">
         <v>1</v>
@@ -1445,10 +1394,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B52" s="3">
-        <v>72304</v>
+        <v>71279.044416608842</v>
       </c>
       <c r="C52" s="4">
         <v>1</v>
@@ -1457,10 +1406,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B53" s="3">
-        <v>71279.044416608842</v>
+        <v>71045.437236189377</v>
       </c>
       <c r="C53" s="4">
         <v>1</v>
@@ -1469,10 +1418,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B54" s="3">
-        <v>71045.437236189377</v>
+        <v>68801.596510717645</v>
       </c>
       <c r="C54" s="4">
         <v>1</v>
@@ -1481,10 +1430,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B55" s="3">
-        <v>68801.596510717645</v>
+        <v>66178</v>
       </c>
       <c r="C55" s="4">
         <v>1</v>
@@ -1493,10 +1442,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B56" s="3">
-        <v>67508.67747857995</v>
+        <v>65936.829161201429</v>
       </c>
       <c r="C56" s="4">
         <v>1</v>
@@ -1505,10 +1454,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B57" s="3">
-        <v>66178</v>
+        <v>65350.6</v>
       </c>
       <c r="C57" s="4">
         <v>1</v>
@@ -1517,10 +1466,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B58" s="3">
-        <v>65936.829161201429</v>
+        <v>58754.554557901625</v>
       </c>
       <c r="C58" s="4">
         <v>1</v>
@@ -1529,10 +1478,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B59" s="3">
-        <v>65350.6</v>
+        <v>55978.568292450909</v>
       </c>
       <c r="C59" s="4">
         <v>1</v>
@@ -1541,10 +1490,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="B60" s="3">
-        <v>58754.554557901625</v>
+        <v>55781.748168259932</v>
       </c>
       <c r="C60" s="4">
         <v>1</v>
@@ -1553,10 +1502,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B61" s="3">
-        <v>55978.568292450909</v>
+        <v>53236.399999999994</v>
       </c>
       <c r="C61" s="4">
         <v>1</v>
@@ -1565,10 +1514,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B62" s="3">
-        <v>55781.748168259932</v>
+        <v>48615.600000000006</v>
       </c>
       <c r="C62" s="4">
         <v>1</v>
@@ -1577,10 +1526,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B63" s="3">
-        <v>53236.399999999994</v>
+        <v>47130.70440228939</v>
       </c>
       <c r="C63" s="4">
         <v>1</v>
@@ -1589,10 +1538,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B64" s="3">
-        <v>48615.600000000006</v>
+        <v>45612.352414952475</v>
       </c>
       <c r="C64" s="4">
         <v>1</v>
@@ -1601,10 +1550,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B65" s="3">
-        <v>47130.70440228939</v>
+        <v>44509.516262606776</v>
       </c>
       <c r="C65" s="4">
         <v>1</v>
@@ -1613,10 +1562,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B66" s="3">
-        <v>45612.352414952475</v>
+        <v>42403.198614379697</v>
       </c>
       <c r="C66" s="4">
         <v>1</v>
@@ -1625,10 +1574,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B67" s="3">
-        <v>44509.516262606776</v>
+        <v>41592.459680903834</v>
       </c>
       <c r="C67" s="4">
         <v>1</v>
@@ -1637,10 +1586,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B68" s="3">
-        <v>42403.198614379697</v>
+        <v>41430.383244903285</v>
       </c>
       <c r="C68" s="4">
         <v>1</v>
@@ -1649,10 +1598,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B69" s="3">
-        <v>41592.459680903834</v>
+        <v>39612.484515818447</v>
       </c>
       <c r="C69" s="4">
         <v>1</v>
@@ -1661,10 +1610,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B70" s="3">
-        <v>41430.383244903285</v>
+        <v>37816</v>
       </c>
       <c r="C70" s="4">
         <v>1</v>
@@ -1673,10 +1622,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B71" s="3">
-        <v>39612.484515818447</v>
+        <v>37343.200000000004</v>
       </c>
       <c r="C71" s="4">
         <v>1</v>
@@ -1685,10 +1634,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B72" s="3">
-        <v>37816</v>
+        <v>37088.484579931552</v>
       </c>
       <c r="C72" s="4">
         <v>1</v>
@@ -1697,10 +1646,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B73" s="3">
-        <v>37343.200000000004</v>
+        <v>37088.48457993153</v>
       </c>
       <c r="C73" s="4">
         <v>1</v>
@@ -1709,10 +1658,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B74" s="3">
-        <v>37088.484579931552</v>
+        <v>35762.163434948663</v>
       </c>
       <c r="C74" s="4">
         <v>1</v>
@@ -1721,10 +1670,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B75" s="3">
-        <v>37088.48457993153</v>
+        <v>35762.163434948634</v>
       </c>
       <c r="C75" s="4">
         <v>1</v>
@@ -1733,10 +1682,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B76" s="3">
-        <v>35762.163434948663</v>
+        <v>35481.353006894577</v>
       </c>
       <c r="C76" s="4">
         <v>1</v>
@@ -1745,10 +1694,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B77" s="3">
-        <v>35762.163434948634</v>
+        <v>33217.576403841915</v>
       </c>
       <c r="C77" s="4">
         <v>1</v>
@@ -1757,10 +1706,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B78" s="3">
-        <v>35481.353006894577</v>
+        <v>32586</v>
       </c>
       <c r="C78" s="4">
         <v>1</v>
@@ -1769,10 +1718,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B79" s="3">
-        <v>33217.576403841915</v>
+        <v>30420.800000000003</v>
       </c>
       <c r="C79" s="4">
         <v>1</v>
@@ -1781,226 +1730,228 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B80" s="3">
-        <v>32586</v>
+        <v>29281.503377839501</v>
       </c>
       <c r="C80" s="4">
         <v>1</v>
       </c>
       <c r="D80"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B81" s="3">
-        <v>30420.800000000003</v>
+        <v>29141.286038496473</v>
       </c>
       <c r="C81" s="4">
         <v>1</v>
       </c>
       <c r="D81"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B82" s="3">
-        <v>29281.503377839501</v>
+        <v>26718.876238633235</v>
       </c>
       <c r="C82" s="4">
         <v>1</v>
       </c>
       <c r="D82"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B83" s="3">
-        <v>29141.286038496473</v>
+        <v>21436.052816368232</v>
       </c>
       <c r="C83" s="4">
         <v>1</v>
       </c>
       <c r="D83"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B84" s="3">
-        <v>26718.876238633235</v>
+        <v>20596.627243388237</v>
       </c>
       <c r="C84" s="4">
         <v>1</v>
       </c>
       <c r="D84"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B85" s="3">
-        <v>21436.052816368232</v>
+        <v>19508</v>
       </c>
       <c r="C85" s="4">
         <v>1</v>
       </c>
       <c r="D85"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B86" s="3">
-        <v>20596.627243388237</v>
+        <v>18062.983557381482</v>
       </c>
       <c r="C86" s="4">
         <v>1</v>
       </c>
       <c r="D86"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="B87" s="3">
-        <v>19508</v>
+        <v>17537.295581713413</v>
       </c>
       <c r="C87" s="4">
         <v>1</v>
       </c>
       <c r="D87"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B88" s="3">
-        <v>18062.983557381482</v>
+        <v>16826.122601439787</v>
       </c>
       <c r="C88" s="4">
         <v>1</v>
       </c>
       <c r="D88"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B89" s="3">
-        <v>17537.295581713413</v>
+        <v>16634.400000000001</v>
       </c>
       <c r="C89" s="4">
         <v>1</v>
       </c>
       <c r="D89"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B90" s="3">
-        <v>16826.122601439787</v>
+        <v>15928.499999999998</v>
       </c>
       <c r="C90" s="4">
         <v>1</v>
       </c>
       <c r="D90"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B91" s="3">
-        <v>16634.400000000001</v>
+        <v>14262.918822015883</v>
       </c>
       <c r="C91" s="4">
         <v>1</v>
       </c>
       <c r="D91"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B92" s="3">
-        <v>15928.499999999998</v>
+        <v>13119.245591411502</v>
       </c>
       <c r="C92" s="4">
         <v>1</v>
       </c>
       <c r="D92"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B93" s="3">
-        <v>14262.918822015883</v>
+        <v>9068.9813571231753</v>
       </c>
       <c r="C93" s="4">
         <v>1</v>
       </c>
       <c r="D93"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B94" s="3">
-        <v>13119.245591411502</v>
+        <v>5849.0172573820937</v>
       </c>
       <c r="C94" s="4">
         <v>1</v>
       </c>
       <c r="D94"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B95" s="3">
-        <v>9068.9813571231753</v>
+        <v>3367.7219768398677</v>
       </c>
       <c r="C95" s="4">
         <v>1</v>
       </c>
       <c r="D95"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="B96" s="3">
-        <v>5849.0172573820937</v>
+        <v>1760200</v>
       </c>
       <c r="C96" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D96"/>
+      <c r="E96" s="2"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B97" s="3">
-        <v>3367.7219768398677</v>
+        <v>1109491.3</v>
       </c>
       <c r="C97" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D97"/>
+      <c r="E97" s="2"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B98" s="3">
-        <v>1760200</v>
+        <v>1003500</v>
       </c>
       <c r="C98" s="4">
         <v>5</v>
@@ -2010,10 +1961,10 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B99" s="3">
-        <v>1109491.3</v>
+        <v>747500</v>
       </c>
       <c r="C99" s="4">
         <v>5</v>
@@ -2026,7 +1977,7 @@
         <v>47</v>
       </c>
       <c r="B100" s="3">
-        <v>1003500</v>
+        <v>630100</v>
       </c>
       <c r="C100" s="4">
         <v>5</v>
@@ -2039,7 +1990,7 @@
         <v>43</v>
       </c>
       <c r="B101" s="3">
-        <v>747500</v>
+        <v>547705.5</v>
       </c>
       <c r="C101" s="4">
         <v>5</v>
@@ -2052,7 +2003,7 @@
         <v>49</v>
       </c>
       <c r="B102" s="3">
-        <v>630100</v>
+        <v>536908.5</v>
       </c>
       <c r="C102" s="4">
         <v>5</v>
@@ -2062,10 +2013,10 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B103" s="3">
-        <v>547705.5</v>
+        <v>424600</v>
       </c>
       <c r="C103" s="4">
         <v>5</v>
@@ -2075,10 +2026,10 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B104" s="3">
-        <v>536908.5</v>
+        <v>374691.65</v>
       </c>
       <c r="C104" s="4">
         <v>5</v>
@@ -2088,10 +2039,10 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B105" s="3">
-        <v>424600</v>
+        <v>322300</v>
       </c>
       <c r="C105" s="4">
         <v>5</v>
@@ -2101,10 +2052,10 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B106" s="3">
-        <v>374691.65</v>
+        <v>277638.37</v>
       </c>
       <c r="C106" s="4">
         <v>5</v>
@@ -2117,7 +2068,7 @@
         <v>48</v>
       </c>
       <c r="B107" s="3">
-        <v>322300</v>
+        <v>274690.02</v>
       </c>
       <c r="C107" s="4">
         <v>5</v>
@@ -2127,10 +2078,10 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B108" s="3">
-        <v>277638.37</v>
+        <v>273003.81</v>
       </c>
       <c r="C108" s="4">
         <v>5</v>
@@ -2140,10 +2091,10 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B109" s="3">
-        <v>274690.02</v>
+        <v>271300</v>
       </c>
       <c r="C109" s="4">
         <v>5</v>
@@ -2153,10 +2104,10 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B110" s="3">
-        <v>273003.81</v>
+        <v>263794.5</v>
       </c>
       <c r="C110" s="4">
         <v>5</v>
@@ -2166,10 +2117,10 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B111" s="3">
-        <v>271300</v>
+        <v>263200</v>
       </c>
       <c r="C111" s="4">
         <v>5</v>
@@ -2179,10 +2130,10 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B112" s="3">
-        <v>263794.5</v>
+        <v>250795</v>
       </c>
       <c r="C112" s="4">
         <v>5</v>
@@ -2195,7 +2146,7 @@
         <v>56</v>
       </c>
       <c r="B113" s="3">
-        <v>263200</v>
+        <v>227700</v>
       </c>
       <c r="C113" s="4">
         <v>5</v>
@@ -2205,10 +2156,10 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="B114" s="3">
-        <v>250795</v>
+        <v>209794.5</v>
       </c>
       <c r="C114" s="4">
         <v>5</v>
@@ -2218,10 +2169,10 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="B115" s="3">
-        <v>227700</v>
+        <v>202484.09</v>
       </c>
       <c r="C115" s="4">
         <v>5</v>
@@ -2231,10 +2182,10 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="B116" s="3">
-        <v>209794.5</v>
+        <v>192992.39</v>
       </c>
       <c r="C116" s="4">
         <v>5</v>
@@ -2244,10 +2195,10 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B117" s="3">
-        <v>202484.09</v>
+        <v>183909.98</v>
       </c>
       <c r="C117" s="4">
         <v>5</v>
@@ -2257,10 +2208,10 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="B118" s="3">
-        <v>192992.39</v>
+        <v>180999.24</v>
       </c>
       <c r="C118" s="4">
         <v>5</v>
@@ -2270,10 +2221,10 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="B119" s="3">
-        <v>183909.98</v>
+        <v>170000</v>
       </c>
       <c r="C119" s="4">
         <v>5</v>
@@ -2283,10 +2234,10 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B120" s="3">
-        <v>180999.24</v>
+        <v>166733.16</v>
       </c>
       <c r="C120" s="4">
         <v>5</v>
@@ -2296,10 +2247,10 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B121" s="3">
-        <v>170000</v>
+        <v>147473.4</v>
       </c>
       <c r="C121" s="4">
         <v>5</v>
@@ -2309,10 +2260,10 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="B122" s="3">
-        <v>166733.16</v>
+        <v>142526.6</v>
       </c>
       <c r="C122" s="4">
         <v>5</v>
@@ -2322,10 +2273,10 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="B123" s="3">
-        <v>147473.4</v>
+        <v>136111.26</v>
       </c>
       <c r="C123" s="4">
         <v>5</v>
@@ -2335,10 +2286,10 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B124" s="3">
-        <v>142526.6</v>
+        <v>132616.46</v>
       </c>
       <c r="C124" s="4">
         <v>5</v>
@@ -2348,10 +2299,10 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B125" s="3">
-        <v>136111.26</v>
+        <v>123200</v>
       </c>
       <c r="C125" s="4">
         <v>5</v>
@@ -2361,10 +2312,10 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B126" s="3">
-        <v>132616.46</v>
+        <v>120621.5</v>
       </c>
       <c r="C126" s="4">
         <v>5</v>
@@ -2374,10 +2325,10 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="B127" s="3">
-        <v>123200</v>
+        <v>119881.81</v>
       </c>
       <c r="C127" s="4">
         <v>5</v>
@@ -2387,10 +2338,10 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B128" s="3">
-        <v>120621.5</v>
+        <v>113273</v>
       </c>
       <c r="C128" s="4">
         <v>5</v>
@@ -2400,10 +2351,10 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="B129" s="3">
-        <v>119881.81</v>
+        <v>110507.61</v>
       </c>
       <c r="C129" s="4">
         <v>5</v>
@@ -2413,10 +2364,10 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B130" s="3">
-        <v>113273</v>
+        <v>106397.5</v>
       </c>
       <c r="C130" s="4">
         <v>5</v>
@@ -2426,10 +2377,10 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B131" s="3">
-        <v>110507.61</v>
+        <v>105380.71</v>
       </c>
       <c r="C131" s="4">
         <v>5</v>
@@ -2439,36 +2390,38 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="B132" s="3">
-        <v>106397.5</v>
+        <v>102500</v>
       </c>
       <c r="C132" s="4">
         <v>5</v>
       </c>
       <c r="D132"/>
       <c r="E132" s="2"/>
+      <c r="H132"/>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="B133" s="3">
-        <v>105380.71</v>
+        <v>102300</v>
       </c>
       <c r="C133" s="4">
         <v>5</v>
       </c>
       <c r="D133"/>
       <c r="E133" s="2"/>
+      <c r="H133"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B134" s="3">
-        <v>102500</v>
+        <v>100000</v>
       </c>
       <c r="C134" s="4">
         <v>5</v>
@@ -2482,7 +2435,7 @@
         <v>103</v>
       </c>
       <c r="B135" s="3">
-        <v>102300</v>
+        <v>97605.063999999998</v>
       </c>
       <c r="C135" s="4">
         <v>5</v>
@@ -2496,7 +2449,7 @@
         <v>104</v>
       </c>
       <c r="B136" s="3">
-        <v>100000</v>
+        <v>91800</v>
       </c>
       <c r="C136" s="4">
         <v>5</v>
@@ -2507,10 +2460,10 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="B137" s="3">
-        <v>97605.063999999998</v>
+        <v>87500</v>
       </c>
       <c r="C137" s="4">
         <v>5</v>
@@ -2521,10 +2474,10 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="B138" s="3">
-        <v>91800</v>
+        <v>87500</v>
       </c>
       <c r="C138" s="4">
         <v>5</v>
@@ -2535,10 +2488,10 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="B139" s="3">
-        <v>87500</v>
+        <v>82500</v>
       </c>
       <c r="C139" s="4">
         <v>5</v>
@@ -2549,10 +2502,10 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B140" s="3">
-        <v>87500</v>
+        <v>81794.334000000003</v>
       </c>
       <c r="C140" s="4">
         <v>5</v>
@@ -2563,10 +2516,10 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B141" s="3">
-        <v>82500</v>
+        <v>81400</v>
       </c>
       <c r="C141" s="4">
         <v>5</v>
@@ -2577,10 +2530,10 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="B142" s="3">
-        <v>81794.334000000003</v>
+        <v>80500</v>
       </c>
       <c r="C142" s="4">
         <v>5</v>
@@ -2591,10 +2544,10 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="B143" s="3">
-        <v>81400</v>
+        <v>77500</v>
       </c>
       <c r="C143" s="4">
         <v>5</v>
@@ -2605,10 +2558,10 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>109</v>
+        <v>71</v>
       </c>
       <c r="B144" s="3">
-        <v>80500</v>
+        <v>75118.187000000005</v>
       </c>
       <c r="C144" s="4">
         <v>5</v>
@@ -2619,10 +2572,10 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="B145" s="3">
-        <v>77500</v>
+        <v>75000</v>
       </c>
       <c r="C145" s="4">
         <v>5</v>
@@ -2633,10 +2586,10 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B146" s="3">
-        <v>75118.187000000005</v>
+        <v>71500</v>
       </c>
       <c r="C146" s="4">
         <v>5</v>
@@ -2647,10 +2600,10 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="B147" s="3">
-        <v>75000</v>
+        <v>69492.385999999999</v>
       </c>
       <c r="C147" s="4">
         <v>5</v>
@@ -2661,10 +2614,10 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="B148" s="3">
-        <v>71500</v>
+        <v>69309.298999999999</v>
       </c>
       <c r="C148" s="4">
         <v>5</v>
@@ -2675,10 +2628,10 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B149" s="3">
-        <v>69492.385999999999</v>
+        <v>62500</v>
       </c>
       <c r="C149" s="4">
         <v>5</v>
@@ -2689,10 +2642,10 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="B150" s="3">
-        <v>69309.298999999999</v>
+        <v>60118.186999999998</v>
       </c>
       <c r="C150" s="4">
         <v>5</v>
@@ -2703,10 +2656,10 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B151" s="3">
-        <v>62500</v>
+        <v>58799.237000000001</v>
       </c>
       <c r="C151" s="4">
         <v>5</v>
@@ -2717,10 +2670,10 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B152" s="3">
-        <v>60118.186999999998</v>
+        <v>57200</v>
       </c>
       <c r="C152" s="4">
         <v>5</v>
@@ -2731,10 +2684,10 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B153" s="3">
-        <v>58799.237000000001</v>
+        <v>57003.807000000001</v>
       </c>
       <c r="C153" s="4">
         <v>5</v>
@@ -2745,10 +2698,10 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="B154" s="3">
-        <v>57200</v>
+        <v>56250</v>
       </c>
       <c r="C154" s="4">
         <v>5</v>
@@ -2759,10 +2712,10 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="B155" s="3">
-        <v>57003.807000000001</v>
+        <v>56100</v>
       </c>
       <c r="C155" s="4">
         <v>5</v>
@@ -2773,10 +2726,10 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>111</v>
+        <v>72</v>
       </c>
       <c r="B156" s="3">
-        <v>56250</v>
+        <v>55508</v>
       </c>
       <c r="C156" s="4">
         <v>5</v>
@@ -2787,10 +2740,10 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B157" s="3">
-        <v>56100</v>
+        <v>52000</v>
       </c>
       <c r="C157" s="4">
         <v>5</v>
@@ -2801,10 +2754,10 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="B158" s="3">
-        <v>55508</v>
+        <v>49000</v>
       </c>
       <c r="C158" s="4">
         <v>5</v>
@@ -2815,10 +2768,10 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="B159" s="3">
-        <v>52000</v>
+        <v>47007.614000000001</v>
       </c>
       <c r="C159" s="4">
         <v>5</v>
@@ -2829,10 +2782,10 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="B160" s="3">
-        <v>49000</v>
+        <v>45068.192999999999</v>
       </c>
       <c r="C160" s="4">
         <v>5</v>
@@ -2843,10 +2796,10 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B161" s="3">
-        <v>47007.614000000001</v>
+        <v>41000</v>
       </c>
       <c r="C161" s="4">
         <v>5</v>
@@ -2857,10 +2810,10 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="B162" s="3">
-        <v>45068.192999999999</v>
+        <v>40887.345999999998</v>
       </c>
       <c r="C162" s="4">
         <v>5</v>
@@ -2874,7 +2827,7 @@
         <v>114</v>
       </c>
       <c r="B163" s="3">
-        <v>41000</v>
+        <v>39600</v>
       </c>
       <c r="C163" s="4">
         <v>5</v>
@@ -2885,10 +2838,10 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="B164" s="3">
-        <v>40887.345999999998</v>
+        <v>37500</v>
       </c>
       <c r="C164" s="4">
         <v>5</v>
@@ -2899,10 +2852,10 @@
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B165" s="3">
-        <v>39600</v>
+        <v>37500</v>
       </c>
       <c r="C165" s="4">
         <v>5</v>
@@ -2913,10 +2866,10 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="B166" s="3">
-        <v>37500</v>
+        <v>36000</v>
       </c>
       <c r="C166" s="4">
         <v>5</v>
@@ -2927,10 +2880,10 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="B167" s="3">
-        <v>37500</v>
+        <v>34100</v>
       </c>
       <c r="C167" s="4">
         <v>5</v>
@@ -2941,10 +2894,10 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B168" s="3">
-        <v>36000</v>
+        <v>30087.514999999999</v>
       </c>
       <c r="C168" s="4">
         <v>5</v>
@@ -2955,10 +2908,10 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="B169" s="3">
-        <v>34100</v>
+        <v>25880.714</v>
       </c>
       <c r="C169" s="4">
         <v>5</v>
@@ -2972,7 +2925,7 @@
         <v>119</v>
       </c>
       <c r="B170" s="3">
-        <v>30087.514999999999</v>
+        <v>25300</v>
       </c>
       <c r="C170" s="4">
         <v>5</v>
@@ -2986,7 +2939,7 @@
         <v>120</v>
       </c>
       <c r="B171" s="3">
-        <v>25880.714</v>
+        <v>24180.714</v>
       </c>
       <c r="C171" s="4">
         <v>5</v>
@@ -3000,7 +2953,7 @@
         <v>121</v>
       </c>
       <c r="B172" s="3">
-        <v>25300</v>
+        <v>23800</v>
       </c>
       <c r="C172" s="4">
         <v>5</v>
@@ -3014,7 +2967,7 @@
         <v>122</v>
       </c>
       <c r="B173" s="3">
-        <v>24180.714</v>
+        <v>22100</v>
       </c>
       <c r="C173" s="4">
         <v>5</v>
@@ -3025,10 +2978,10 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
       <c r="B174" s="3">
-        <v>23800</v>
+        <v>21445.96</v>
       </c>
       <c r="C174" s="4">
         <v>5</v>
@@ -3039,10 +2992,10 @@
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B175" s="3">
-        <v>22100</v>
+        <v>20439.145</v>
       </c>
       <c r="C175" s="4">
         <v>5</v>
@@ -3053,10 +3006,10 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="B176" s="3">
-        <v>21445.96</v>
+        <v>15473.308000000001</v>
       </c>
       <c r="C176" s="4">
         <v>5</v>
@@ -3067,10 +3020,10 @@
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
       <c r="B177" s="3">
-        <v>20439.145</v>
+        <v>11750</v>
       </c>
       <c r="C177" s="4">
         <v>5</v>
@@ -3081,10 +3034,10 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B178" s="3">
-        <v>15473.308000000001</v>
+        <v>10955.665999999999</v>
       </c>
       <c r="C178" s="4">
         <v>5</v>
@@ -3095,10 +3048,10 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B179" s="3">
-        <v>11750</v>
+        <v>9500</v>
       </c>
       <c r="C179" s="4">
         <v>5</v>
@@ -3109,10 +3062,10 @@
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B180" s="3">
-        <v>10955.665999999999</v>
+        <v>8396.1929999999993</v>
       </c>
       <c r="C180" s="4">
         <v>5</v>
@@ -3123,10 +3076,10 @@
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B181" s="3">
-        <v>9500</v>
+        <v>6496.1930000000002</v>
       </c>
       <c r="C181" s="4">
         <v>5</v>
@@ -3137,10 +3090,10 @@
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="B182" s="3">
-        <v>8396.1929999999993</v>
+        <v>5000</v>
       </c>
       <c r="C182" s="4">
         <v>5</v>
@@ -3151,10 +3104,10 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="B183" s="3">
-        <v>6496.1930000000002</v>
+        <v>5000</v>
       </c>
       <c r="C183" s="4">
         <v>5</v>
@@ -3165,10 +3118,10 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
       <c r="B184" s="3">
-        <v>5000</v>
+        <v>4024.5862999999999</v>
       </c>
       <c r="C184" s="4">
         <v>5</v>
@@ -3179,10 +3132,10 @@
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="B185" s="3">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="C185" s="4">
         <v>5</v>
@@ -3193,223 +3146,96 @@
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B186" s="3">
-        <v>4024.5862999999999</v>
+        <v>794.33435999999995</v>
       </c>
       <c r="C186" s="4">
         <v>5</v>
       </c>
       <c r="D186"/>
       <c r="E186" s="2"/>
-      <c r="H186"/>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A187" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B187" s="3">
-        <v>2500</v>
-      </c>
-      <c r="C187" s="4">
-        <v>5</v>
-      </c>
-      <c r="D187"/>
-      <c r="E187" s="2"/>
-      <c r="H187"/>
+      <c r="B187" s="7"/>
+      <c r="C187" s="4"/>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A188" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B188" s="3">
-        <v>794.33435999999995</v>
-      </c>
-      <c r="C188" s="4">
-        <v>5</v>
-      </c>
-      <c r="D188"/>
-      <c r="E188" s="2"/>
+      <c r="B188" s="7"/>
+      <c r="C188" s="4"/>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A189" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B189" s="7">
-        <v>300000</v>
-      </c>
-      <c r="C189" s="4">
-        <v>5</v>
-      </c>
+      <c r="B189" s="7"/>
+      <c r="C189" s="4"/>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A190" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B190" s="7">
-        <v>150000</v>
-      </c>
-      <c r="C190" s="4">
-        <v>5</v>
-      </c>
+      <c r="B190" s="7"/>
+      <c r="C190" s="4"/>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A191" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B191" s="7">
-        <v>600000</v>
-      </c>
-      <c r="C191" s="4">
-        <v>5</v>
-      </c>
+      <c r="B191" s="7"/>
+      <c r="C191" s="4"/>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A192" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B192" s="7">
-        <v>150000</v>
-      </c>
-      <c r="C192" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B193" s="7">
-        <v>150000</v>
-      </c>
-      <c r="C193" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B194" s="7">
-        <v>300000</v>
-      </c>
-      <c r="C194" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B195" s="7">
-        <v>150000</v>
-      </c>
-      <c r="C195" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B196" s="7">
-        <v>600000</v>
-      </c>
-      <c r="C196" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B197" s="7">
-        <v>150000</v>
-      </c>
-      <c r="C197" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B198" s="7">
-        <v>300000</v>
-      </c>
-      <c r="C198" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B199" s="7">
-        <v>150000</v>
-      </c>
-      <c r="C199" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B200" s="7">
-        <v>450000</v>
-      </c>
-      <c r="C200" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B201" s="7">
-        <v>150000</v>
-      </c>
-      <c r="C201" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B202" s="7">
-        <v>150000</v>
-      </c>
-      <c r="C202" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A203" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B203" s="7">
-        <v>300000</v>
-      </c>
-      <c r="C203" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B192" s="7"/>
+      <c r="C192" s="4"/>
+    </row>
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B193" s="7"/>
+      <c r="C193" s="4"/>
+    </row>
+    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B194" s="7"/>
+      <c r="C194" s="4"/>
+    </row>
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B195" s="7"/>
+      <c r="C195" s="4"/>
+    </row>
+    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B196" s="7"/>
+      <c r="C196" s="4"/>
+    </row>
+    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B197" s="7"/>
+      <c r="C197" s="4"/>
+    </row>
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B198" s="7"/>
+      <c r="C198" s="4"/>
+    </row>
+    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B199" s="7"/>
+      <c r="C199" s="4"/>
+    </row>
+    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B200" s="7"/>
+      <c r="C200" s="4"/>
+    </row>
+    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B201" s="7"/>
+      <c r="C201" s="4"/>
+    </row>
+    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B202" s="3"/>
+    </row>
+    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B203" s="3"/>
+    </row>
+    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204" s="3"/>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" s="3"/>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" s="3"/>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" s="3"/>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" s="3"/>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.25">
@@ -18672,12 +18498,6 @@
     </row>
     <row r="5295" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5295" s="3"/>
-    </row>
-    <row r="5296" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5296" s="3"/>
-    </row>
-    <row r="5297" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5297" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>